<commit_message>
Added chronic user chart
</commit_message>
<xml_diff>
--- a/2 - Heroin/h.xlsx
+++ b/2 - Heroin/h.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25540" windowHeight="21140" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19160" windowHeight="21140" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="INFO" sheetId="5" r:id="rId1"/>
@@ -113,18 +113,6 @@
     <t>2010-2011</t>
   </si>
   <si>
-    <t>21+ days in past month</t>
-  </si>
-  <si>
-    <t>11–20 days in past month</t>
-  </si>
-  <si>
-    <t>4–10 days in past month</t>
-  </si>
-  <si>
-    <t>Chronic (10 or more days)</t>
-  </si>
-  <si>
     <t xml:space="preserve">  Female</t>
   </si>
   <si>
@@ -144,6 +132,18 @@
   </si>
   <si>
     <t>Year</t>
+  </si>
+  <si>
+    <t>Occasional Users</t>
+  </si>
+  <si>
+    <t>Chronic Users (more than 10 days per/mo)</t>
+  </si>
+  <si>
+    <t>HerionUseByFrequency</t>
+  </si>
+  <si>
+    <t>National, Thousands</t>
   </si>
 </sst>
 </file>
@@ -715,10 +715,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:B3"/>
+  <dimension ref="A2:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -729,18 +729,26 @@
   <sheetData>
     <row r="2" spans="1:2">
       <c r="A2" s="12" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
         <v>25</v>
+      </c>
+      <c r="B4" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -760,8 +768,8 @@
   </sheetPr>
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -771,13 +779,13 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="14" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -961,7 +969,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1107,225 +1115,145 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="2" max="2" width="14.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="45">
+    <row r="1" spans="1:3" ht="75">
       <c r="A1" s="10"/>
       <c r="B1" s="10" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D1" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="E1" s="10" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" s="9">
         <v>2000</v>
       </c>
       <c r="B2" s="9">
-        <v>0.3</v>
+        <v>170</v>
       </c>
       <c r="C2" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="D2" s="9">
-        <v>0.9</v>
-      </c>
-      <c r="E2" s="9">
-        <f>C2+D2</f>
-        <v>1.1000000000000001</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
+        <v>1400</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" s="9">
         <v>2001</v>
       </c>
       <c r="B3" s="9">
-        <v>0.3</v>
+        <v>130</v>
       </c>
       <c r="C3" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="D3" s="9">
-        <v>0.9</v>
-      </c>
-      <c r="E3" s="9">
-        <f t="shared" ref="E3:E12" si="0">C3+D3</f>
-        <v>1.1000000000000001</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
+        <v>1400</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4" s="9">
         <v>2002</v>
       </c>
       <c r="B4" s="9">
-        <v>0.2</v>
+        <v>210</v>
       </c>
       <c r="C4" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="D4" s="9">
-        <v>0.9</v>
-      </c>
-      <c r="E4" s="9">
-        <f t="shared" si="0"/>
-        <v>1.1000000000000001</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
+        <v>1300</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5" s="9">
         <v>2003</v>
       </c>
       <c r="B5" s="9">
-        <v>0.2</v>
+        <v>130</v>
       </c>
       <c r="C5" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="D5" s="9">
-        <v>0.9</v>
-      </c>
-      <c r="E5" s="9">
-        <f t="shared" si="0"/>
-        <v>1.1000000000000001</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
+        <v>1300</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6" s="9">
         <v>2004</v>
       </c>
       <c r="B6" s="9">
-        <v>0.2</v>
+        <v>120</v>
       </c>
       <c r="C6" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="D6" s="9">
-        <v>0.9</v>
-      </c>
-      <c r="E6" s="9">
-        <f t="shared" si="0"/>
-        <v>1.1000000000000001</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
+        <v>1300</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
       <c r="A7" s="9">
         <v>2005</v>
       </c>
       <c r="B7" s="9">
-        <v>0.2</v>
+        <v>180</v>
       </c>
       <c r="C7" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="D7" s="9">
-        <v>0.8</v>
-      </c>
-      <c r="E7" s="9">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
       <c r="A8" s="9">
         <v>2006</v>
       </c>
       <c r="B8" s="9">
-        <v>0.2</v>
+        <v>380</v>
       </c>
       <c r="C8" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="D8" s="9">
-        <v>0.8</v>
-      </c>
-      <c r="E8" s="9">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
       <c r="A9" s="9">
         <v>2007</v>
       </c>
       <c r="B9" s="9">
-        <v>0.2</v>
+        <v>150</v>
       </c>
       <c r="C9" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="D9" s="9">
-        <v>0.8</v>
-      </c>
-      <c r="E9" s="9">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
       <c r="A10" s="9">
         <v>2008</v>
       </c>
       <c r="B10" s="9">
-        <v>0.2</v>
+        <v>240</v>
       </c>
       <c r="C10" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="D10" s="9">
-        <v>0.9</v>
-      </c>
-      <c r="E10" s="9">
-        <f t="shared" si="0"/>
-        <v>1.1000000000000001</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
+        <v>1300</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
       <c r="A11" s="9">
         <v>2009</v>
       </c>
       <c r="B11" s="9">
-        <v>0.3</v>
+        <v>340</v>
       </c>
       <c r="C11" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="D11" s="9">
-        <v>1</v>
-      </c>
-      <c r="E11" s="9">
-        <f t="shared" si="0"/>
-        <v>1.2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
       <c r="A12" s="9">
         <v>2010</v>
       </c>
       <c r="B12" s="9">
-        <v>0.3</v>
+        <v>330</v>
       </c>
       <c r="C12" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="D12" s="9">
-        <v>1</v>
-      </c>
-      <c r="E12" s="9">
-        <f t="shared" si="0"/>
-        <v>1.2</v>
+        <v>1500</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Got a working Choropleth
</commit_message>
<xml_diff>
--- a/2 - Heroin/h.xlsx
+++ b/2 - Heroin/h.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38320" windowHeight="21140" tabRatio="660"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="26500" windowHeight="21140" tabRatio="660" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="INFO" sheetId="5" r:id="rId1"/>
@@ -17,7 +17,7 @@
     <sheet name="Prevalence" sheetId="8" r:id="rId8"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">Prevalence!$A$1:$G$137</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">Prevalence!$A$1:$L$137</definedName>
   </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="622" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="873" uniqueCount="444">
   <si>
     <t>RACE</t>
   </si>
@@ -786,6 +786,633 @@
   </si>
   <si>
     <t>Opioid Use Prevalence</t>
+  </si>
+  <si>
+    <t xml:space="preserve">['Country', </t>
+  </si>
+  <si>
+    <t>Prevalence]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">['Kenya', </t>
+  </si>
+  <si>
+    <t>0.21],</t>
+  </si>
+  <si>
+    <t xml:space="preserve">['Mauritius', </t>
+  </si>
+  <si>
+    <t>1.29],</t>
+  </si>
+  <si>
+    <t xml:space="preserve">['Rwanda', </t>
+  </si>
+  <si>
+    <t>0.14],</t>
+  </si>
+  <si>
+    <t xml:space="preserve">['Seychelles', </t>
+  </si>
+  <si>
+    <t>2.3],</t>
+  </si>
+  <si>
+    <t xml:space="preserve">['Somalia', </t>
+  </si>
+  <si>
+    <t>0.16],</t>
+  </si>
+  <si>
+    <t xml:space="preserve">['Uganda', </t>
+  </si>
+  <si>
+    <t>0.05],</t>
+  </si>
+  <si>
+    <t xml:space="preserve">['Algeria', </t>
+  </si>
+  <si>
+    <t>0.06],</t>
+  </si>
+  <si>
+    <t xml:space="preserve">['Egypt', </t>
+  </si>
+  <si>
+    <t>0.44],</t>
+  </si>
+  <si>
+    <t xml:space="preserve">['Libya', </t>
+  </si>
+  <si>
+    <t xml:space="preserve">['Morocco', </t>
+  </si>
+  <si>
+    <t>0.08],</t>
+  </si>
+  <si>
+    <t xml:space="preserve">['Tunisia', </t>
+  </si>
+  <si>
+    <t>0.12],</t>
+  </si>
+  <si>
+    <t xml:space="preserve">['South Africa', </t>
+  </si>
+  <si>
+    <t>0.5],</t>
+  </si>
+  <si>
+    <t xml:space="preserve">['Swaziland', </t>
+  </si>
+  <si>
+    <t>0.17],</t>
+  </si>
+  <si>
+    <t xml:space="preserve">['Zambia', </t>
+  </si>
+  <si>
+    <t>0.37],</t>
+  </si>
+  <si>
+    <t xml:space="preserve">['Zimbabwe', </t>
+  </si>
+  <si>
+    <t>0.04],</t>
+  </si>
+  <si>
+    <t xml:space="preserve">['Central African Republic', </t>
+  </si>
+  <si>
+    <t xml:space="preserve">['Chad', </t>
+  </si>
+  <si>
+    <t>0.22],</t>
+  </si>
+  <si>
+    <t xml:space="preserve">['Cabo Verde', </t>
+  </si>
+  <si>
+    <t>0.18],</t>
+  </si>
+  <si>
+    <t xml:space="preserve">['Ghana', </t>
+  </si>
+  <si>
+    <t xml:space="preserve">['Liberia', </t>
+  </si>
+  <si>
+    <t xml:space="preserve">['Niger', </t>
+  </si>
+  <si>
+    <t>0.2],</t>
+  </si>
+  <si>
+    <t xml:space="preserve">['Nigeria', </t>
+  </si>
+  <si>
+    <t>0.7],</t>
+  </si>
+  <si>
+    <t xml:space="preserve">['Congo', </t>
+  </si>
+  <si>
+    <t>0.13],</t>
+  </si>
+  <si>
+    <t xml:space="preserve">['Senegal', </t>
+  </si>
+  <si>
+    <t xml:space="preserve">['Sierra Leone', </t>
+  </si>
+  <si>
+    <t xml:space="preserve">['Democratic Republic of the Congo', </t>
+  </si>
+  <si>
+    <t xml:space="preserve">['Barbados', </t>
+  </si>
+  <si>
+    <t>0.23],</t>
+  </si>
+  <si>
+    <t xml:space="preserve">['Bermuda', </t>
+  </si>
+  <si>
+    <t>0.15],</t>
+  </si>
+  <si>
+    <t xml:space="preserve">['Bahamas', </t>
+  </si>
+  <si>
+    <t xml:space="preserve">['Dominican Republic', </t>
+  </si>
+  <si>
+    <t>0.07],</t>
+  </si>
+  <si>
+    <t xml:space="preserve">['Haiti', </t>
+  </si>
+  <si>
+    <t xml:space="preserve">['Jamaica', </t>
+  </si>
+  <si>
+    <t>1],</t>
+  </si>
+  <si>
+    <t xml:space="preserve">['Belize', </t>
+  </si>
+  <si>
+    <t>0.3],</t>
+  </si>
+  <si>
+    <t xml:space="preserve">['Costa Rica', </t>
+  </si>
+  <si>
+    <t>0.63],</t>
+  </si>
+  <si>
+    <t xml:space="preserve">['El Salvador', </t>
+  </si>
+  <si>
+    <t xml:space="preserve">['Guatemala', </t>
+  </si>
+  <si>
+    <t xml:space="preserve">['Honduras', </t>
+  </si>
+  <si>
+    <t xml:space="preserve">['Nicaragua', </t>
+  </si>
+  <si>
+    <t>0.02],</t>
+  </si>
+  <si>
+    <t xml:space="preserve">['Canada', </t>
+  </si>
+  <si>
+    <t xml:space="preserve">['Mexico', </t>
+  </si>
+  <si>
+    <t>0.38],</t>
+  </si>
+  <si>
+    <t xml:space="preserve">['United States of America', </t>
+  </si>
+  <si>
+    <t>6.1],</t>
+  </si>
+  <si>
+    <t xml:space="preserve">['Argentina', </t>
+  </si>
+  <si>
+    <t>0.1],</t>
+  </si>
+  <si>
+    <t xml:space="preserve">['Bolivia (Plurinational State of)', </t>
+  </si>
+  <si>
+    <t>0.6],</t>
+  </si>
+  <si>
+    <t xml:space="preserve">['Brazil', </t>
+  </si>
+  <si>
+    <t>1.45],</t>
+  </si>
+  <si>
+    <t xml:space="preserve">['Chile', </t>
+  </si>
+  <si>
+    <t>0.28],</t>
+  </si>
+  <si>
+    <t xml:space="preserve">['Colombia', </t>
+  </si>
+  <si>
+    <t xml:space="preserve">['Ecuador', </t>
+  </si>
+  <si>
+    <t xml:space="preserve">['Paraguay', </t>
+  </si>
+  <si>
+    <t>0.03],</t>
+  </si>
+  <si>
+    <t xml:space="preserve">['Peru', </t>
+  </si>
+  <si>
+    <t xml:space="preserve">['Suriname', </t>
+  </si>
+  <si>
+    <t xml:space="preserve">['Uruguay', </t>
+  </si>
+  <si>
+    <t xml:space="preserve">['Venezuela (Bolivarian Republic of)', </t>
+  </si>
+  <si>
+    <t xml:space="preserve">['Armenia', </t>
+  </si>
+  <si>
+    <t xml:space="preserve">['Azerbaijan', </t>
+  </si>
+  <si>
+    <t>1.5],</t>
+  </si>
+  <si>
+    <t xml:space="preserve">['Georgia', </t>
+  </si>
+  <si>
+    <t>1.36],</t>
+  </si>
+  <si>
+    <t xml:space="preserve">['Kazakhstan', </t>
+  </si>
+  <si>
+    <t xml:space="preserve">['Kyrgyzstan', </t>
+  </si>
+  <si>
+    <t>0.8],</t>
+  </si>
+  <si>
+    <t xml:space="preserve">['Tajikistan', </t>
+  </si>
+  <si>
+    <t>0.54],</t>
+  </si>
+  <si>
+    <t xml:space="preserve">['Turkmenistan', </t>
+  </si>
+  <si>
+    <t>0.32],</t>
+  </si>
+  <si>
+    <t xml:space="preserve">['Uzbekistan', </t>
+  </si>
+  <si>
+    <t xml:space="preserve">['Cambodia', </t>
+  </si>
+  <si>
+    <t xml:space="preserve">['China', </t>
+  </si>
+  <si>
+    <t>0.19],</t>
+  </si>
+  <si>
+    <t xml:space="preserve">['China, Hong Kong SAR', </t>
+  </si>
+  <si>
+    <t xml:space="preserve">['Indonesia', </t>
+  </si>
+  <si>
+    <t>0.11],</t>
+  </si>
+  <si>
+    <t xml:space="preserve">['Lao People's Democratic Republic', </t>
+  </si>
+  <si>
+    <t xml:space="preserve">['China, Macao SAR', </t>
+  </si>
+  <si>
+    <t>1.12],</t>
+  </si>
+  <si>
+    <t xml:space="preserve">['Malaysia', </t>
+  </si>
+  <si>
+    <t>0.94],</t>
+  </si>
+  <si>
+    <t xml:space="preserve">['Mongolia', </t>
+  </si>
+  <si>
+    <t xml:space="preserve">['Myanmar', </t>
+  </si>
+  <si>
+    <t xml:space="preserve">['Philippines', </t>
+  </si>
+  <si>
+    <t xml:space="preserve">['Republic of Korea', </t>
+  </si>
+  <si>
+    <t xml:space="preserve">['Singapore', </t>
+  </si>
+  <si>
+    <t>0.33],</t>
+  </si>
+  <si>
+    <t xml:space="preserve">['Thailand', </t>
+  </si>
+  <si>
+    <t xml:space="preserve">['Timor-Leste', </t>
+  </si>
+  <si>
+    <t xml:space="preserve">['Viet Nam', </t>
+  </si>
+  <si>
+    <t>0.53],</t>
+  </si>
+  <si>
+    <t xml:space="preserve">['Taiwan Province of China', </t>
+  </si>
+  <si>
+    <t xml:space="preserve">['Afghanistan', </t>
+  </si>
+  <si>
+    <t>2.92],</t>
+  </si>
+  <si>
+    <t xml:space="preserve">['Iran (Islamic Republic of)', </t>
+  </si>
+  <si>
+    <t>2.27],</t>
+  </si>
+  <si>
+    <t xml:space="preserve">['Israel', </t>
+  </si>
+  <si>
+    <t xml:space="preserve">['Kuwait', </t>
+  </si>
+  <si>
+    <t xml:space="preserve">['Lebanon', </t>
+  </si>
+  <si>
+    <t xml:space="preserve">['Oman', </t>
+  </si>
+  <si>
+    <t xml:space="preserve">['Pakistan', </t>
+  </si>
+  <si>
+    <t>2.4],</t>
+  </si>
+  <si>
+    <t xml:space="preserve">['Saudi Arabia', </t>
+  </si>
+  <si>
+    <t xml:space="preserve">['Syrian Arab Republic', </t>
+  </si>
+  <si>
+    <t xml:space="preserve">['United Arab Emirates', </t>
+  </si>
+  <si>
+    <t xml:space="preserve">['Bangladesh', </t>
+  </si>
+  <si>
+    <t>0.4],</t>
+  </si>
+  <si>
+    <t xml:space="preserve">['Maldives', </t>
+  </si>
+  <si>
+    <t>1.46],</t>
+  </si>
+  <si>
+    <t xml:space="preserve">['Nepal', </t>
+  </si>
+  <si>
+    <t>0.24],</t>
+  </si>
+  <si>
+    <t xml:space="preserve">['Sri Lanka', </t>
+  </si>
+  <si>
+    <t xml:space="preserve">['Belarus', </t>
+  </si>
+  <si>
+    <t>0.59],</t>
+  </si>
+  <si>
+    <t xml:space="preserve">['Republic of Moldova', </t>
+  </si>
+  <si>
+    <t xml:space="preserve">['Russian Federation', </t>
+  </si>
+  <si>
+    <t>1.64],</t>
+  </si>
+  <si>
+    <t xml:space="preserve">['Ukraine', </t>
+  </si>
+  <si>
+    <t>0.91],</t>
+  </si>
+  <si>
+    <t xml:space="preserve">['Albania', </t>
+  </si>
+  <si>
+    <t>0.45],</t>
+  </si>
+  <si>
+    <t xml:space="preserve">['Bosnia and Herzegovina', </t>
+  </si>
+  <si>
+    <t xml:space="preserve">['Bulgaria', </t>
+  </si>
+  <si>
+    <t>0.51],</t>
+  </si>
+  <si>
+    <t xml:space="preserve">['Croatia', </t>
+  </si>
+  <si>
+    <t>0.36],</t>
+  </si>
+  <si>
+    <t xml:space="preserve">['The former Yugoslav Republic of Macedonia', </t>
+  </si>
+  <si>
+    <t xml:space="preserve">['Romania', </t>
+  </si>
+  <si>
+    <t xml:space="preserve">['Turkey', </t>
+  </si>
+  <si>
+    <t xml:space="preserve">['Serbia', </t>
+  </si>
+  <si>
+    <t xml:space="preserve">['Austria', </t>
+  </si>
+  <si>
+    <t xml:space="preserve">['Belgium', </t>
+  </si>
+  <si>
+    <t xml:space="preserve">['Cyprus', </t>
+  </si>
+  <si>
+    <t xml:space="preserve">['Czech Republic', </t>
+  </si>
+  <si>
+    <t>2.7],</t>
+  </si>
+  <si>
+    <t xml:space="preserve">['Denmark', </t>
+  </si>
+  <si>
+    <t>0.52],</t>
+  </si>
+  <si>
+    <t xml:space="preserve">['Estonia', </t>
+  </si>
+  <si>
+    <t>1.53],</t>
+  </si>
+  <si>
+    <t xml:space="preserve">['Finland', </t>
+  </si>
+  <si>
+    <t xml:space="preserve">['France', </t>
+  </si>
+  <si>
+    <t>0.49],</t>
+  </si>
+  <si>
+    <t xml:space="preserve">['Germany', </t>
+  </si>
+  <si>
+    <t xml:space="preserve">['Greece', </t>
+  </si>
+  <si>
+    <t>0.29],</t>
+  </si>
+  <si>
+    <t xml:space="preserve">['Hungary', </t>
+  </si>
+  <si>
+    <t xml:space="preserve">['Iceland', </t>
+  </si>
+  <si>
+    <t xml:space="preserve">['Ireland', </t>
+  </si>
+  <si>
+    <t>0.72],</t>
+  </si>
+  <si>
+    <t xml:space="preserve">['Italy', </t>
+  </si>
+  <si>
+    <t xml:space="preserve">['Latvia', </t>
+  </si>
+  <si>
+    <t>0.66],</t>
+  </si>
+  <si>
+    <t xml:space="preserve">['Liechtenstein', </t>
+  </si>
+  <si>
+    <t xml:space="preserve">['Lithuania', </t>
+  </si>
+  <si>
+    <t xml:space="preserve">['Luxembourg', </t>
+  </si>
+  <si>
+    <t xml:space="preserve">['Malta', </t>
+  </si>
+  <si>
+    <t>0.62],</t>
+  </si>
+  <si>
+    <t xml:space="preserve">['Monaco', </t>
+  </si>
+  <si>
+    <t xml:space="preserve">['Netherlands', </t>
+  </si>
+  <si>
+    <t xml:space="preserve">['Norway', </t>
+  </si>
+  <si>
+    <t xml:space="preserve">['Poland', </t>
+  </si>
+  <si>
+    <t xml:space="preserve">['Portugal', </t>
+  </si>
+  <si>
+    <t xml:space="preserve">['Slovenia', </t>
+  </si>
+  <si>
+    <t xml:space="preserve">['Slovakia', </t>
+  </si>
+  <si>
+    <t xml:space="preserve">['Spain', </t>
+  </si>
+  <si>
+    <t xml:space="preserve">['Sweden', </t>
+  </si>
+  <si>
+    <t xml:space="preserve">['Switzerland', </t>
+  </si>
+  <si>
+    <t xml:space="preserve">['United Kingdom (England and Wales)', </t>
+  </si>
+  <si>
+    <t>0.73],</t>
+  </si>
+  <si>
+    <t xml:space="preserve">['United Kingdom (Northern Ireland)', </t>
+  </si>
+  <si>
+    <t xml:space="preserve">['United Kingdom (Scotland)', </t>
+  </si>
+  <si>
+    <t>1.71],</t>
+  </si>
+  <si>
+    <t xml:space="preserve">['Australia', </t>
+  </si>
+  <si>
+    <t>3.4],</t>
+  </si>
+  <si>
+    <t xml:space="preserve">['New Zealand', </t>
+  </si>
+  <si>
+    <t>1.1],</t>
+  </si>
+  <si>
+    <t>value1</t>
+  </si>
+  <si>
+    <t>value2</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ],</t>
   </si>
 </sst>
 </file>
@@ -885,7 +1512,7 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -916,8 +1543,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -1073,8 +1706,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="59">
+  <cellStyleXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1134,8 +1776,32 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1211,8 +1877,17 @@
     <xf numFmtId="0" fontId="12" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="59">
+  <cellStyles count="83">
     <cellStyle name="Comma 2" xfId="46"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -1242,6 +1917,18 @@
     <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1270,6 +1957,18 @@
     <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="45"/>
   </cellStyles>
@@ -1602,7 +2301,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
@@ -2436,11 +3135,11 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G162"/>
+  <dimension ref="A1:L138"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
+      <selection pane="bottomLeft" activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2451,11 +3150,12 @@
     <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="5.33203125" customWidth="1"/>
     <col min="6" max="6" width="7" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="30.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="2.83203125" customWidth="1"/>
+    <col min="7" max="7" width="30.5" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="7" customWidth="1"/>
+    <col min="9" max="9" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="25" customHeight="1">
+    <row r="1" spans="1:12" ht="28">
       <c r="A1" s="19" t="s">
         <v>50</v>
       </c>
@@ -2477,8 +3177,21 @@
       <c r="G1" s="22" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="2" spans="1:7">
+      <c r="H1" s="35"/>
+      <c r="I1" s="36" t="s">
+        <v>235</v>
+      </c>
+      <c r="J1" s="36" t="s">
+        <v>236</v>
+      </c>
+      <c r="K1" s="35" t="s">
+        <v>441</v>
+      </c>
+      <c r="L1" s="35" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
       <c r="A2" s="33" t="s">
         <v>52</v>
       </c>
@@ -2500,8 +3213,26 @@
       <c r="G2" s="26" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="3" spans="1:7">
+      <c r="H2" s="37" t="str">
+        <f>"'"</f>
+        <v>'</v>
+      </c>
+      <c r="I2" t="str">
+        <f>CONCATENATE("[",H2,A2,H2,", ")</f>
+        <v xml:space="preserve">['Kenya', </v>
+      </c>
+      <c r="J2" t="str">
+        <f>CONCATENATE(B2,"],")</f>
+        <v>0.21],</v>
+      </c>
+      <c r="K2" t="s">
+        <v>237</v>
+      </c>
+      <c r="L2" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
       <c r="A3" s="33" t="s">
         <v>58</v>
       </c>
@@ -2519,8 +3250,26 @@
       <c r="G3" s="26" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="4" spans="1:7">
+      <c r="H3" s="37" t="str">
+        <f t="shared" ref="H3:H66" si="0">"'"</f>
+        <v>'</v>
+      </c>
+      <c r="I3" t="str">
+        <f t="shared" ref="I3:I66" si="1">CONCATENATE("[",H3,A3,H3,", ")</f>
+        <v xml:space="preserve">['Mauritius', </v>
+      </c>
+      <c r="J3" t="str">
+        <f t="shared" ref="J3:J66" si="2">CONCATENATE(B3,"],")</f>
+        <v>1.29],</v>
+      </c>
+      <c r="K3" t="s">
+        <v>239</v>
+      </c>
+      <c r="L3" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
       <c r="A4" s="33" t="s">
         <v>63</v>
       </c>
@@ -2538,8 +3287,26 @@
       <c r="G4" s="26" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="5" spans="1:7">
+      <c r="H4" s="37" t="str">
+        <f t="shared" si="0"/>
+        <v>'</v>
+      </c>
+      <c r="I4" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">['Rwanda', </v>
+      </c>
+      <c r="J4" t="str">
+        <f t="shared" si="2"/>
+        <v>0.14],</v>
+      </c>
+      <c r="K4" t="s">
+        <v>241</v>
+      </c>
+      <c r="L4" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
       <c r="A5" s="33" t="s">
         <v>65</v>
       </c>
@@ -2557,8 +3324,26 @@
       <c r="G5" s="26" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="6" spans="1:7">
+      <c r="H5" s="37" t="str">
+        <f t="shared" si="0"/>
+        <v>'</v>
+      </c>
+      <c r="I5" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">['Seychelles', </v>
+      </c>
+      <c r="J5" t="str">
+        <f t="shared" si="2"/>
+        <v>2.3],</v>
+      </c>
+      <c r="K5" t="s">
+        <v>243</v>
+      </c>
+      <c r="L5" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
       <c r="A6" s="33" t="s">
         <v>68</v>
       </c>
@@ -2576,8 +3361,26 @@
       <c r="G6" s="26" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="7" spans="1:7">
+      <c r="H6" s="37" t="str">
+        <f t="shared" si="0"/>
+        <v>'</v>
+      </c>
+      <c r="I6" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">['Somalia', </v>
+      </c>
+      <c r="J6" t="str">
+        <f t="shared" si="2"/>
+        <v>0.16],</v>
+      </c>
+      <c r="K6" t="s">
+        <v>245</v>
+      </c>
+      <c r="L6" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
       <c r="A7" s="33" t="s">
         <v>69</v>
       </c>
@@ -2595,8 +3398,26 @@
       <c r="G7" s="26" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="8" spans="1:7">
+      <c r="H7" s="37" t="str">
+        <f t="shared" si="0"/>
+        <v>'</v>
+      </c>
+      <c r="I7" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">['Uganda', </v>
+      </c>
+      <c r="J7" t="str">
+        <f t="shared" si="2"/>
+        <v>0.05],</v>
+      </c>
+      <c r="K7" t="s">
+        <v>247</v>
+      </c>
+      <c r="L7" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
       <c r="A8" s="33" t="s">
         <v>70</v>
       </c>
@@ -2618,8 +3439,26 @@
       <c r="G8" s="26" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="9" spans="1:7">
+      <c r="H8" s="37" t="str">
+        <f t="shared" si="0"/>
+        <v>'</v>
+      </c>
+      <c r="I8" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">['Algeria', </v>
+      </c>
+      <c r="J8" t="str">
+        <f t="shared" si="2"/>
+        <v>0.06],</v>
+      </c>
+      <c r="K8" t="s">
+        <v>249</v>
+      </c>
+      <c r="L8" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
       <c r="A9" s="33" t="s">
         <v>74</v>
       </c>
@@ -2641,8 +3480,26 @@
       <c r="G9" s="26" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="10" spans="1:7">
+      <c r="H9" s="37" t="str">
+        <f t="shared" si="0"/>
+        <v>'</v>
+      </c>
+      <c r="I9" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">['Egypt', </v>
+      </c>
+      <c r="J9" t="str">
+        <f t="shared" si="2"/>
+        <v>0.44],</v>
+      </c>
+      <c r="K9" t="s">
+        <v>251</v>
+      </c>
+      <c r="L9" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
       <c r="A10" s="33" t="s">
         <v>77</v>
       </c>
@@ -2660,8 +3517,26 @@
       <c r="G10" s="26" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="11" spans="1:7">
+      <c r="H10" s="37" t="str">
+        <f t="shared" si="0"/>
+        <v>'</v>
+      </c>
+      <c r="I10" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">['Libya', </v>
+      </c>
+      <c r="J10" t="str">
+        <f t="shared" si="2"/>
+        <v>0.14],</v>
+      </c>
+      <c r="K10" t="s">
+        <v>253</v>
+      </c>
+      <c r="L10" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
       <c r="A11" s="33" t="s">
         <v>78</v>
       </c>
@@ -2679,8 +3554,26 @@
       <c r="G11" s="26" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="12" spans="1:7">
+      <c r="H11" s="37" t="str">
+        <f t="shared" si="0"/>
+        <v>'</v>
+      </c>
+      <c r="I11" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">['Morocco', </v>
+      </c>
+      <c r="J11" t="str">
+        <f t="shared" si="2"/>
+        <v>0.08],</v>
+      </c>
+      <c r="K11" t="s">
+        <v>254</v>
+      </c>
+      <c r="L11" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
       <c r="A12" s="33" t="s">
         <v>80</v>
       </c>
@@ -2698,8 +3591,26 @@
       <c r="G12" s="26" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="13" spans="1:7">
+      <c r="H12" s="37" t="str">
+        <f t="shared" si="0"/>
+        <v>'</v>
+      </c>
+      <c r="I12" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">['Tunisia', </v>
+      </c>
+      <c r="J12" t="str">
+        <f t="shared" si="2"/>
+        <v>0.12],</v>
+      </c>
+      <c r="K12" t="s">
+        <v>256</v>
+      </c>
+      <c r="L12" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
       <c r="A13" s="33" t="s">
         <v>81</v>
       </c>
@@ -2717,8 +3628,26 @@
       <c r="G13" s="26" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="14" spans="1:7">
+      <c r="H13" s="37" t="str">
+        <f t="shared" si="0"/>
+        <v>'</v>
+      </c>
+      <c r="I13" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">['South Africa', </v>
+      </c>
+      <c r="J13" t="str">
+        <f t="shared" si="2"/>
+        <v>0.5],</v>
+      </c>
+      <c r="K13" t="s">
+        <v>258</v>
+      </c>
+      <c r="L13" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
       <c r="A14" s="33" t="s">
         <v>83</v>
       </c>
@@ -2736,8 +3665,26 @@
       <c r="G14" s="26" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="15" spans="1:7">
+      <c r="H14" s="37" t="str">
+        <f t="shared" si="0"/>
+        <v>'</v>
+      </c>
+      <c r="I14" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">['Swaziland', </v>
+      </c>
+      <c r="J14" t="str">
+        <f t="shared" si="2"/>
+        <v>0.17],</v>
+      </c>
+      <c r="K14" t="s">
+        <v>260</v>
+      </c>
+      <c r="L14" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
       <c r="A15" s="33" t="s">
         <v>84</v>
       </c>
@@ -2755,8 +3702,26 @@
       <c r="G15" s="26" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="16" spans="1:7">
+      <c r="H15" s="37" t="str">
+        <f t="shared" si="0"/>
+        <v>'</v>
+      </c>
+      <c r="I15" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">['Zambia', </v>
+      </c>
+      <c r="J15" t="str">
+        <f t="shared" si="2"/>
+        <v>0.37],</v>
+      </c>
+      <c r="K15" t="s">
+        <v>262</v>
+      </c>
+      <c r="L15" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12">
       <c r="A16" s="33" t="s">
         <v>85</v>
       </c>
@@ -2774,8 +3739,26 @@
       <c r="G16" s="26" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="17" spans="1:7">
+      <c r="H16" s="37" t="str">
+        <f t="shared" si="0"/>
+        <v>'</v>
+      </c>
+      <c r="I16" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">['Zimbabwe', </v>
+      </c>
+      <c r="J16" t="str">
+        <f t="shared" si="2"/>
+        <v>0.04],</v>
+      </c>
+      <c r="K16" t="s">
+        <v>264</v>
+      </c>
+      <c r="L16" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12">
       <c r="A17" s="33" t="s">
         <v>86</v>
       </c>
@@ -2793,8 +3776,26 @@
       <c r="G17" s="26" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="18" spans="1:7">
+      <c r="H17" s="37" t="str">
+        <f t="shared" si="0"/>
+        <v>'</v>
+      </c>
+      <c r="I17" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">['Central African Republic', </v>
+      </c>
+      <c r="J17" t="str">
+        <f t="shared" si="2"/>
+        <v>0.05],</v>
+      </c>
+      <c r="K17" t="s">
+        <v>266</v>
+      </c>
+      <c r="L17" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12">
       <c r="A18" s="33" t="s">
         <v>87</v>
       </c>
@@ -2812,8 +3813,26 @@
       <c r="G18" s="26" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="19" spans="1:7">
+      <c r="H18" s="37" t="str">
+        <f t="shared" si="0"/>
+        <v>'</v>
+      </c>
+      <c r="I18" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">['Chad', </v>
+      </c>
+      <c r="J18" t="str">
+        <f t="shared" si="2"/>
+        <v>0.22],</v>
+      </c>
+      <c r="K18" t="s">
+        <v>267</v>
+      </c>
+      <c r="L18" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12">
       <c r="A19" s="33" t="s">
         <v>88</v>
       </c>
@@ -2831,8 +3850,26 @@
       <c r="G19" s="26" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="20" spans="1:7">
+      <c r="H19" s="37" t="str">
+        <f t="shared" si="0"/>
+        <v>'</v>
+      </c>
+      <c r="I19" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">['Cabo Verde', </v>
+      </c>
+      <c r="J19" t="str">
+        <f t="shared" si="2"/>
+        <v>0.18],</v>
+      </c>
+      <c r="K19" t="s">
+        <v>269</v>
+      </c>
+      <c r="L19" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12">
       <c r="A20" s="33" t="s">
         <v>89</v>
       </c>
@@ -2850,8 +3887,26 @@
       <c r="G20" s="26" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="21" spans="1:7">
+      <c r="H20" s="37" t="str">
+        <f t="shared" si="0"/>
+        <v>'</v>
+      </c>
+      <c r="I20" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">['Ghana', </v>
+      </c>
+      <c r="J20" t="str">
+        <f t="shared" si="2"/>
+        <v>0.14],</v>
+      </c>
+      <c r="K20" t="s">
+        <v>271</v>
+      </c>
+      <c r="L20" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12">
       <c r="A21" s="33" t="s">
         <v>91</v>
       </c>
@@ -2869,8 +3924,26 @@
       <c r="G21" s="26" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" ht="28">
+      <c r="H21" s="37" t="str">
+        <f t="shared" si="0"/>
+        <v>'</v>
+      </c>
+      <c r="I21" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">['Liberia', </v>
+      </c>
+      <c r="J21" t="str">
+        <f t="shared" si="2"/>
+        <v>0.17],</v>
+      </c>
+      <c r="K21" t="s">
+        <v>272</v>
+      </c>
+      <c r="L21" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="15" customHeight="1">
       <c r="A22" s="33" t="s">
         <v>92</v>
       </c>
@@ -2888,8 +3961,26 @@
       <c r="G22" s="26" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="23" spans="1:7">
+      <c r="H22" s="37" t="str">
+        <f t="shared" si="0"/>
+        <v>'</v>
+      </c>
+      <c r="I22" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">['Niger', </v>
+      </c>
+      <c r="J22" t="str">
+        <f t="shared" si="2"/>
+        <v>0.2],</v>
+      </c>
+      <c r="K22" t="s">
+        <v>273</v>
+      </c>
+      <c r="L22" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12">
       <c r="A23" s="33" t="s">
         <v>93</v>
       </c>
@@ -2911,8 +4002,26 @@
       <c r="G23" s="26" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="24" spans="1:7">
+      <c r="H23" s="37" t="str">
+        <f t="shared" si="0"/>
+        <v>'</v>
+      </c>
+      <c r="I23" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">['Nigeria', </v>
+      </c>
+      <c r="J23" t="str">
+        <f t="shared" si="2"/>
+        <v>0.7],</v>
+      </c>
+      <c r="K23" t="s">
+        <v>275</v>
+      </c>
+      <c r="L23" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12">
       <c r="A24" s="33" t="s">
         <v>94</v>
       </c>
@@ -2930,8 +4039,26 @@
       <c r="G24" s="26" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="25" spans="1:7">
+      <c r="H24" s="37" t="str">
+        <f t="shared" si="0"/>
+        <v>'</v>
+      </c>
+      <c r="I24" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">['Congo', </v>
+      </c>
+      <c r="J24" t="str">
+        <f t="shared" si="2"/>
+        <v>0.13],</v>
+      </c>
+      <c r="K24" t="s">
+        <v>277</v>
+      </c>
+      <c r="L24" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12">
       <c r="A25" s="33" t="s">
         <v>95</v>
       </c>
@@ -2949,8 +4076,26 @@
       <c r="G25" s="26" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="26" spans="1:7">
+      <c r="H25" s="37" t="str">
+        <f t="shared" si="0"/>
+        <v>'</v>
+      </c>
+      <c r="I25" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">['Senegal', </v>
+      </c>
+      <c r="J25" t="str">
+        <f t="shared" si="2"/>
+        <v>0.08],</v>
+      </c>
+      <c r="K25" t="s">
+        <v>279</v>
+      </c>
+      <c r="L25" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12">
       <c r="A26" s="33" t="s">
         <v>96</v>
       </c>
@@ -2968,8 +4113,26 @@
       <c r="G26" s="26" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" ht="23" customHeight="1">
+      <c r="H26" s="37" t="str">
+        <f t="shared" si="0"/>
+        <v>'</v>
+      </c>
+      <c r="I26" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">['Sierra Leone', </v>
+      </c>
+      <c r="J26" t="str">
+        <f t="shared" si="2"/>
+        <v>0.17],</v>
+      </c>
+      <c r="K26" t="s">
+        <v>280</v>
+      </c>
+      <c r="L26" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12">
       <c r="A27" s="33" t="s">
         <v>97</v>
       </c>
@@ -2987,8 +4150,26 @@
       <c r="G27" s="26" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="28" spans="1:7">
+      <c r="H27" s="37" t="str">
+        <f t="shared" si="0"/>
+        <v>'</v>
+      </c>
+      <c r="I27" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">['Democratic Republic of the Congo', </v>
+      </c>
+      <c r="J27" t="str">
+        <f t="shared" si="2"/>
+        <v>0.17],</v>
+      </c>
+      <c r="K27" t="s">
+        <v>281</v>
+      </c>
+      <c r="L27" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12">
       <c r="A28" s="33" t="s">
         <v>98</v>
       </c>
@@ -3010,8 +4191,26 @@
       <c r="G28" s="26" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="29" spans="1:7">
+      <c r="H28" s="37" t="str">
+        <f t="shared" si="0"/>
+        <v>'</v>
+      </c>
+      <c r="I28" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">['Barbados', </v>
+      </c>
+      <c r="J28" t="str">
+        <f t="shared" si="2"/>
+        <v>0.23],</v>
+      </c>
+      <c r="K28" t="s">
+        <v>282</v>
+      </c>
+      <c r="L28" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12">
       <c r="A29" s="33" t="s">
         <v>99</v>
       </c>
@@ -3033,8 +4232,26 @@
       <c r="G29" s="26" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="30" spans="1:7">
+      <c r="H29" s="37" t="str">
+        <f t="shared" si="0"/>
+        <v>'</v>
+      </c>
+      <c r="I29" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">['Bermuda', </v>
+      </c>
+      <c r="J29" t="str">
+        <f t="shared" si="2"/>
+        <v>0.15],</v>
+      </c>
+      <c r="K29" t="s">
+        <v>284</v>
+      </c>
+      <c r="L29" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12">
       <c r="A30" s="33" t="s">
         <v>101</v>
       </c>
@@ -3052,8 +4269,26 @@
       <c r="G30" s="26" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="31" spans="1:7">
+      <c r="H30" s="37" t="str">
+        <f t="shared" si="0"/>
+        <v>'</v>
+      </c>
+      <c r="I30" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">['Bahamas', </v>
+      </c>
+      <c r="J30" t="str">
+        <f t="shared" si="2"/>
+        <v>0.22],</v>
+      </c>
+      <c r="K30" t="s">
+        <v>286</v>
+      </c>
+      <c r="L30" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12">
       <c r="A31" s="33" t="s">
         <v>102</v>
       </c>
@@ -3075,8 +4310,26 @@
       <c r="G31" s="26" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" ht="18" customHeight="1">
+      <c r="H31" s="37" t="str">
+        <f t="shared" si="0"/>
+        <v>'</v>
+      </c>
+      <c r="I31" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">['Dominican Republic', </v>
+      </c>
+      <c r="J31" t="str">
+        <f t="shared" si="2"/>
+        <v>0.07],</v>
+      </c>
+      <c r="K31" t="s">
+        <v>287</v>
+      </c>
+      <c r="L31" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12">
       <c r="A32" s="33" t="s">
         <v>103</v>
       </c>
@@ -3098,8 +4351,26 @@
       <c r="G32" s="26" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="33" spans="1:7">
+      <c r="H32" s="37" t="str">
+        <f t="shared" si="0"/>
+        <v>'</v>
+      </c>
+      <c r="I32" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">['Haiti', </v>
+      </c>
+      <c r="J32" t="str">
+        <f t="shared" si="2"/>
+        <v>0.2],</v>
+      </c>
+      <c r="K32" t="s">
+        <v>289</v>
+      </c>
+      <c r="L32" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12">
       <c r="A33" s="33" t="s">
         <v>104</v>
       </c>
@@ -3121,8 +4392,26 @@
       <c r="G33" s="26" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="34" spans="1:7">
+      <c r="H33" s="37" t="str">
+        <f t="shared" si="0"/>
+        <v>'</v>
+      </c>
+      <c r="I33" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">['Jamaica', </v>
+      </c>
+      <c r="J33" t="str">
+        <f t="shared" si="2"/>
+        <v>1],</v>
+      </c>
+      <c r="K33" t="s">
+        <v>290</v>
+      </c>
+      <c r="L33" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12">
       <c r="A34" s="33" t="s">
         <v>105</v>
       </c>
@@ -3140,8 +4429,26 @@
       <c r="G34" s="26" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="35" spans="1:7">
+      <c r="H34" s="37" t="str">
+        <f t="shared" si="0"/>
+        <v>'</v>
+      </c>
+      <c r="I34" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">['Belize', </v>
+      </c>
+      <c r="J34" t="str">
+        <f t="shared" si="2"/>
+        <v>0.3],</v>
+      </c>
+      <c r="K34" t="s">
+        <v>292</v>
+      </c>
+      <c r="L34" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12">
       <c r="A35" s="33" t="s">
         <v>109</v>
       </c>
@@ -3159,8 +4466,26 @@
       <c r="G35" s="26" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="36" spans="1:7">
+      <c r="H35" s="37" t="str">
+        <f t="shared" si="0"/>
+        <v>'</v>
+      </c>
+      <c r="I35" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">['Costa Rica', </v>
+      </c>
+      <c r="J35" t="str">
+        <f t="shared" si="2"/>
+        <v>0.63],</v>
+      </c>
+      <c r="K35" t="s">
+        <v>294</v>
+      </c>
+      <c r="L35" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12">
       <c r="A36" s="33" t="s">
         <v>110</v>
       </c>
@@ -3178,8 +4503,26 @@
       <c r="G36" s="26" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="37" spans="1:7">
+      <c r="H36" s="37" t="str">
+        <f t="shared" si="0"/>
+        <v>'</v>
+      </c>
+      <c r="I36" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">['El Salvador', </v>
+      </c>
+      <c r="J36" t="str">
+        <f t="shared" si="2"/>
+        <v>0.14],</v>
+      </c>
+      <c r="K36" t="s">
+        <v>296</v>
+      </c>
+      <c r="L36" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12">
       <c r="A37" s="33" t="s">
         <v>111</v>
       </c>
@@ -3197,8 +4540,26 @@
       <c r="G37" s="26" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="38" spans="1:7">
+      <c r="H37" s="37" t="str">
+        <f t="shared" si="0"/>
+        <v>'</v>
+      </c>
+      <c r="I37" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">['Guatemala', </v>
+      </c>
+      <c r="J37" t="str">
+        <f t="shared" si="2"/>
+        <v>0.04],</v>
+      </c>
+      <c r="K37" t="s">
+        <v>297</v>
+      </c>
+      <c r="L37" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12">
       <c r="A38" s="33" t="s">
         <v>112</v>
       </c>
@@ -3216,8 +4577,26 @@
       <c r="G38" s="26" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="39" spans="1:7">
+      <c r="H38" s="37" t="str">
+        <f t="shared" si="0"/>
+        <v>'</v>
+      </c>
+      <c r="I38" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">['Honduras', </v>
+      </c>
+      <c r="J38" t="str">
+        <f t="shared" si="2"/>
+        <v>0.15],</v>
+      </c>
+      <c r="K38" t="s">
+        <v>298</v>
+      </c>
+      <c r="L38" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12">
       <c r="A39" s="33" t="s">
         <v>113</v>
       </c>
@@ -3235,8 +4614,26 @@
       <c r="G39" s="26" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="40" spans="1:7">
+      <c r="H39" s="37" t="str">
+        <f t="shared" si="0"/>
+        <v>'</v>
+      </c>
+      <c r="I39" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">['Nicaragua', </v>
+      </c>
+      <c r="J39" t="str">
+        <f t="shared" si="2"/>
+        <v>0.02],</v>
+      </c>
+      <c r="K39" t="s">
+        <v>299</v>
+      </c>
+      <c r="L39" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12">
       <c r="A40" s="33" t="s">
         <v>114</v>
       </c>
@@ -3254,8 +4651,26 @@
       <c r="G40" s="26" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="41" spans="1:7">
+      <c r="H40" s="37" t="str">
+        <f t="shared" si="0"/>
+        <v>'</v>
+      </c>
+      <c r="I40" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">['Canada', </v>
+      </c>
+      <c r="J40" t="str">
+        <f t="shared" si="2"/>
+        <v>0.3],</v>
+      </c>
+      <c r="K40" t="s">
+        <v>301</v>
+      </c>
+      <c r="L40" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12">
       <c r="A41" s="33" t="s">
         <v>115</v>
       </c>
@@ -3277,8 +4692,26 @@
       <c r="G41" s="26" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="42" spans="1:7">
+      <c r="H41" s="37" t="str">
+        <f t="shared" si="0"/>
+        <v>'</v>
+      </c>
+      <c r="I41" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">['Mexico', </v>
+      </c>
+      <c r="J41" t="str">
+        <f t="shared" si="2"/>
+        <v>0.38],</v>
+      </c>
+      <c r="K41" t="s">
+        <v>302</v>
+      </c>
+      <c r="L41" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12">
       <c r="A42" s="33" t="s">
         <v>116</v>
       </c>
@@ -3296,8 +4729,26 @@
       <c r="G42" s="26" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="43" spans="1:7" ht="18" customHeight="1">
+      <c r="H42" s="37" t="str">
+        <f t="shared" si="0"/>
+        <v>'</v>
+      </c>
+      <c r="I42" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">['United States of America', </v>
+      </c>
+      <c r="J42" t="str">
+        <f t="shared" si="2"/>
+        <v>6.1],</v>
+      </c>
+      <c r="K42" t="s">
+        <v>304</v>
+      </c>
+      <c r="L42" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12">
       <c r="A43" s="33" t="s">
         <v>117</v>
       </c>
@@ -3315,8 +4766,26 @@
       <c r="G43" s="26" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="44" spans="1:7">
+      <c r="H43" s="37" t="str">
+        <f t="shared" si="0"/>
+        <v>'</v>
+      </c>
+      <c r="I43" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">['Argentina', </v>
+      </c>
+      <c r="J43" t="str">
+        <f t="shared" si="2"/>
+        <v>0.1],</v>
+      </c>
+      <c r="K43" t="s">
+        <v>306</v>
+      </c>
+      <c r="L43" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12">
       <c r="A44" s="33" t="s">
         <v>118</v>
       </c>
@@ -3338,8 +4807,26 @@
       <c r="G44" s="26" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="45" spans="1:7" ht="18" customHeight="1">
+      <c r="H44" s="37" t="str">
+        <f t="shared" si="0"/>
+        <v>'</v>
+      </c>
+      <c r="I44" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">['Bolivia (Plurinational State of)', </v>
+      </c>
+      <c r="J44" t="str">
+        <f t="shared" si="2"/>
+        <v>0.6],</v>
+      </c>
+      <c r="K44" t="s">
+        <v>308</v>
+      </c>
+      <c r="L44" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12">
       <c r="A45" s="33" t="s">
         <v>119</v>
       </c>
@@ -3361,8 +4848,26 @@
       <c r="G45" s="26" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="46" spans="1:7">
+      <c r="H45" s="37" t="str">
+        <f t="shared" si="0"/>
+        <v>'</v>
+      </c>
+      <c r="I45" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">['Brazil', </v>
+      </c>
+      <c r="J45" t="str">
+        <f t="shared" si="2"/>
+        <v>1.45],</v>
+      </c>
+      <c r="K45" t="s">
+        <v>310</v>
+      </c>
+      <c r="L45" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12">
       <c r="A46" s="33" t="s">
         <v>120</v>
       </c>
@@ -3380,8 +4885,26 @@
       <c r="G46" s="26" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="47" spans="1:7">
+      <c r="H46" s="37" t="str">
+        <f t="shared" si="0"/>
+        <v>'</v>
+      </c>
+      <c r="I46" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">['Chile', </v>
+      </c>
+      <c r="J46" t="str">
+        <f t="shared" si="2"/>
+        <v>0.28],</v>
+      </c>
+      <c r="K46" t="s">
+        <v>312</v>
+      </c>
+      <c r="L46" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12">
       <c r="A47" s="33" t="s">
         <v>121</v>
       </c>
@@ -3399,8 +4922,26 @@
       <c r="G47" s="26" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="48" spans="1:7">
+      <c r="H47" s="37" t="str">
+        <f t="shared" si="0"/>
+        <v>'</v>
+      </c>
+      <c r="I47" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">['Colombia', </v>
+      </c>
+      <c r="J47" t="str">
+        <f t="shared" si="2"/>
+        <v>0.02],</v>
+      </c>
+      <c r="K47" t="s">
+        <v>314</v>
+      </c>
+      <c r="L47" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12">
       <c r="A48" s="33" t="s">
         <v>122</v>
       </c>
@@ -3422,8 +4963,26 @@
       <c r="G48" s="26" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="49" spans="1:7">
+      <c r="H48" s="37" t="str">
+        <f t="shared" si="0"/>
+        <v>'</v>
+      </c>
+      <c r="I48" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">['Ecuador', </v>
+      </c>
+      <c r="J48" t="str">
+        <f t="shared" si="2"/>
+        <v>0.07],</v>
+      </c>
+      <c r="K48" t="s">
+        <v>315</v>
+      </c>
+      <c r="L48" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12">
       <c r="A49" s="33" t="s">
         <v>123</v>
       </c>
@@ -3441,8 +5000,26 @@
       <c r="G49" s="26" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="50" spans="1:7">
+      <c r="H49" s="37" t="str">
+        <f t="shared" si="0"/>
+        <v>'</v>
+      </c>
+      <c r="I49" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">['Paraguay', </v>
+      </c>
+      <c r="J49" t="str">
+        <f t="shared" si="2"/>
+        <v>0.03],</v>
+      </c>
+      <c r="K49" t="s">
+        <v>316</v>
+      </c>
+      <c r="L49" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12">
       <c r="A50" s="33" t="s">
         <v>124</v>
       </c>
@@ -3460,31 +5037,72 @@
       <c r="G50" s="26" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="51" spans="1:7">
+      <c r="H50" s="37" t="str">
+        <f t="shared" si="0"/>
+        <v>'</v>
+      </c>
+      <c r="I50" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">['Peru', </v>
+      </c>
+      <c r="J50" t="str">
+        <f t="shared" si="2"/>
+        <v>0.18],</v>
+      </c>
+      <c r="K50" t="s">
+        <v>318</v>
+      </c>
+      <c r="L50" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12">
       <c r="A51" s="33" t="s">
         <v>126</v>
       </c>
-      <c r="B51" s="23" t="s">
-        <v>51</v>
-      </c>
-      <c r="C51" s="24" t="s">
-        <v>51</v>
-      </c>
-      <c r="D51" s="24" t="s">
-        <v>51</v>
-      </c>
-      <c r="E51" s="25" t="s">
-        <v>51</v>
-      </c>
-      <c r="F51" s="25" t="s">
-        <v>51</v>
+      <c r="B51" s="23" t="str">
+        <f>" "</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="C51" s="23" t="str">
+        <f t="shared" ref="C51:F51" si="3">" "</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="D51" s="23" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="E51" s="23" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="F51" s="23" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="G51" s="26" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="52" spans="1:7">
+      <c r="H51" s="37" t="str">
+        <f t="shared" si="0"/>
+        <v>'</v>
+      </c>
+      <c r="I51" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">['Suriname', </v>
+      </c>
+      <c r="J51" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> ],</v>
+      </c>
+      <c r="K51" t="s">
+        <v>319</v>
+      </c>
+      <c r="L51" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12">
       <c r="A52" s="33" t="s">
         <v>127</v>
       </c>
@@ -3506,8 +5124,26 @@
       <c r="G52" s="26" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="53" spans="1:7">
+      <c r="H52" s="37" t="str">
+        <f t="shared" si="0"/>
+        <v>'</v>
+      </c>
+      <c r="I52" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">['Uruguay', </v>
+      </c>
+      <c r="J52" t="str">
+        <f t="shared" si="2"/>
+        <v>0.18],</v>
+      </c>
+      <c r="K52" t="s">
+        <v>320</v>
+      </c>
+      <c r="L52" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12">
       <c r="A53" s="33" t="s">
         <v>128</v>
       </c>
@@ -3525,8 +5161,26 @@
       <c r="G53" s="26" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="54" spans="1:7">
+      <c r="H53" s="37" t="str">
+        <f t="shared" si="0"/>
+        <v>'</v>
+      </c>
+      <c r="I53" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">['Venezuela (Bolivarian Republic of)', </v>
+      </c>
+      <c r="J53" t="str">
+        <f t="shared" si="2"/>
+        <v>0.03],</v>
+      </c>
+      <c r="K53" t="s">
+        <v>321</v>
+      </c>
+      <c r="L53" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12">
       <c r="A54" s="33" t="s">
         <v>129</v>
       </c>
@@ -3548,8 +5202,26 @@
       <c r="G54" s="26" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="55" spans="1:7">
+      <c r="H54" s="37" t="str">
+        <f t="shared" si="0"/>
+        <v>'</v>
+      </c>
+      <c r="I54" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">['Armenia', </v>
+      </c>
+      <c r="J54" t="str">
+        <f t="shared" si="2"/>
+        <v>0.16],</v>
+      </c>
+      <c r="K54" t="s">
+        <v>322</v>
+      </c>
+      <c r="L54" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12">
       <c r="A55" s="33" t="s">
         <v>131</v>
       </c>
@@ -3571,8 +5243,26 @@
       <c r="G55" s="26" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="56" spans="1:7">
+      <c r="H55" s="37" t="str">
+        <f t="shared" si="0"/>
+        <v>'</v>
+      </c>
+      <c r="I55" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">['Azerbaijan', </v>
+      </c>
+      <c r="J55" t="str">
+        <f t="shared" si="2"/>
+        <v>1.5],</v>
+      </c>
+      <c r="K55" t="s">
+        <v>323</v>
+      </c>
+      <c r="L55" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12">
       <c r="A56" s="33" t="s">
         <v>133</v>
       </c>
@@ -3594,8 +5284,26 @@
       <c r="G56" s="26" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="57" spans="1:7">
+      <c r="H56" s="37" t="str">
+        <f t="shared" si="0"/>
+        <v>'</v>
+      </c>
+      <c r="I56" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">['Georgia', </v>
+      </c>
+      <c r="J56" t="str">
+        <f t="shared" si="2"/>
+        <v>1.36],</v>
+      </c>
+      <c r="K56" t="s">
+        <v>325</v>
+      </c>
+      <c r="L56" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12">
       <c r="A57" s="33" t="s">
         <v>135</v>
       </c>
@@ -3613,8 +5321,26 @@
       <c r="G57" s="26" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="58" spans="1:7">
+      <c r="H57" s="37" t="str">
+        <f t="shared" si="0"/>
+        <v>'</v>
+      </c>
+      <c r="I57" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">['Kazakhstan', </v>
+      </c>
+      <c r="J57" t="str">
+        <f t="shared" si="2"/>
+        <v>1],</v>
+      </c>
+      <c r="K57" t="s">
+        <v>327</v>
+      </c>
+      <c r="L57" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12">
       <c r="A58" s="33" t="s">
         <v>137</v>
       </c>
@@ -3632,8 +5358,26 @@
       <c r="G58" s="26" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="59" spans="1:7">
+      <c r="H58" s="37" t="str">
+        <f t="shared" si="0"/>
+        <v>'</v>
+      </c>
+      <c r="I58" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">['Kyrgyzstan', </v>
+      </c>
+      <c r="J58" t="str">
+        <f t="shared" si="2"/>
+        <v>0.8],</v>
+      </c>
+      <c r="K58" t="s">
+        <v>328</v>
+      </c>
+      <c r="L58" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12">
       <c r="A59" s="33" t="s">
         <v>138</v>
       </c>
@@ -3651,8 +5395,26 @@
       <c r="G59" s="26" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="60" spans="1:7">
+      <c r="H59" s="37" t="str">
+        <f t="shared" si="0"/>
+        <v>'</v>
+      </c>
+      <c r="I59" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">['Tajikistan', </v>
+      </c>
+      <c r="J59" t="str">
+        <f t="shared" si="2"/>
+        <v>0.54],</v>
+      </c>
+      <c r="K59" t="s">
+        <v>330</v>
+      </c>
+      <c r="L59" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12">
       <c r="A60" s="33" t="s">
         <v>139</v>
       </c>
@@ -3670,8 +5432,26 @@
       <c r="G60" s="26" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="61" spans="1:7">
+      <c r="H60" s="37" t="str">
+        <f t="shared" si="0"/>
+        <v>'</v>
+      </c>
+      <c r="I60" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">['Turkmenistan', </v>
+      </c>
+      <c r="J60" t="str">
+        <f t="shared" si="2"/>
+        <v>0.32],</v>
+      </c>
+      <c r="K60" t="s">
+        <v>332</v>
+      </c>
+      <c r="L60" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12">
       <c r="A61" s="33" t="s">
         <v>140</v>
       </c>
@@ -3689,8 +5469,26 @@
       <c r="G61" s="26" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="62" spans="1:7">
+      <c r="H61" s="37" t="str">
+        <f t="shared" si="0"/>
+        <v>'</v>
+      </c>
+      <c r="I61" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">['Uzbekistan', </v>
+      </c>
+      <c r="J61" t="str">
+        <f t="shared" si="2"/>
+        <v>0.8],</v>
+      </c>
+      <c r="K61" t="s">
+        <v>334</v>
+      </c>
+      <c r="L61" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12">
       <c r="A62" s="33" t="s">
         <v>141</v>
       </c>
@@ -3708,8 +5506,26 @@
       <c r="G62" s="26" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="63" spans="1:7">
+      <c r="H62" s="37" t="str">
+        <f t="shared" si="0"/>
+        <v>'</v>
+      </c>
+      <c r="I62" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">['Cambodia', </v>
+      </c>
+      <c r="J62" t="str">
+        <f t="shared" si="2"/>
+        <v>0.04],</v>
+      </c>
+      <c r="K62" t="s">
+        <v>335</v>
+      </c>
+      <c r="L62" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12">
       <c r="A63" s="33" t="s">
         <v>142</v>
       </c>
@@ -3731,8 +5547,26 @@
       <c r="G63" s="26" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="64" spans="1:7">
+      <c r="H63" s="37" t="str">
+        <f t="shared" si="0"/>
+        <v>'</v>
+      </c>
+      <c r="I63" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">['China', </v>
+      </c>
+      <c r="J63" t="str">
+        <f t="shared" si="2"/>
+        <v>0.19],</v>
+      </c>
+      <c r="K63" t="s">
+        <v>336</v>
+      </c>
+      <c r="L63" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12">
       <c r="A64" s="33" t="s">
         <v>144</v>
       </c>
@@ -3750,8 +5584,26 @@
       <c r="G64" s="26" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="65" spans="1:7">
+      <c r="H64" s="37" t="str">
+        <f t="shared" si="0"/>
+        <v>'</v>
+      </c>
+      <c r="I64" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">['China, Hong Kong SAR', </v>
+      </c>
+      <c r="J64" t="str">
+        <f t="shared" si="2"/>
+        <v>0.2],</v>
+      </c>
+      <c r="K64" t="s">
+        <v>338</v>
+      </c>
+      <c r="L64" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12">
       <c r="A65" s="33" t="s">
         <v>145</v>
       </c>
@@ -3769,8 +5621,26 @@
       <c r="G65" s="26" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="66" spans="1:7">
+      <c r="H65" s="37" t="str">
+        <f t="shared" si="0"/>
+        <v>'</v>
+      </c>
+      <c r="I65" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">['Indonesia', </v>
+      </c>
+      <c r="J65" t="str">
+        <f t="shared" si="2"/>
+        <v>0.11],</v>
+      </c>
+      <c r="K65" t="s">
+        <v>339</v>
+      </c>
+      <c r="L65" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12">
       <c r="A66" s="33" t="s">
         <v>146</v>
       </c>
@@ -3788,8 +5658,26 @@
       <c r="G66" s="26" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="67" spans="1:7">
+      <c r="H66" s="37" t="str">
+        <f t="shared" si="0"/>
+        <v>'</v>
+      </c>
+      <c r="I66" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">['Lao People's Democratic Republic', </v>
+      </c>
+      <c r="J66" t="str">
+        <f t="shared" si="2"/>
+        <v>0.37],</v>
+      </c>
+      <c r="K66" t="s">
+        <v>341</v>
+      </c>
+      <c r="L66" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12">
       <c r="A67" s="33" t="s">
         <v>148</v>
       </c>
@@ -3807,8 +5695,26 @@
       <c r="G67" s="26" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="68" spans="1:7" ht="18" customHeight="1">
+      <c r="H67" s="37" t="str">
+        <f t="shared" ref="H67:H130" si="4">"'"</f>
+        <v>'</v>
+      </c>
+      <c r="I67" t="str">
+        <f t="shared" ref="I67:I130" si="5">CONCATENATE("[",H67,A67,H67,", ")</f>
+        <v xml:space="preserve">['China, Macao SAR', </v>
+      </c>
+      <c r="J67" t="str">
+        <f t="shared" ref="J67:J130" si="6">CONCATENATE(B67,"],")</f>
+        <v>1.12],</v>
+      </c>
+      <c r="K67" t="s">
+        <v>342</v>
+      </c>
+      <c r="L67" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12">
       <c r="A68" s="33" t="s">
         <v>149</v>
       </c>
@@ -3826,31 +5732,72 @@
       <c r="G68" s="26" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="69" spans="1:7" ht="18" customHeight="1">
+      <c r="H68" s="37" t="str">
+        <f t="shared" si="4"/>
+        <v>'</v>
+      </c>
+      <c r="I68" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">['Malaysia', </v>
+      </c>
+      <c r="J68" t="str">
+        <f t="shared" si="6"/>
+        <v>0.94],</v>
+      </c>
+      <c r="K68" t="s">
+        <v>344</v>
+      </c>
+      <c r="L68" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12">
       <c r="A69" s="33" t="s">
         <v>151</v>
       </c>
-      <c r="B69" s="23" t="s">
-        <v>51</v>
-      </c>
-      <c r="C69" s="24" t="s">
-        <v>51</v>
-      </c>
-      <c r="D69" s="24" t="s">
-        <v>51</v>
-      </c>
-      <c r="E69" s="25" t="s">
-        <v>51</v>
-      </c>
-      <c r="F69" s="25" t="s">
-        <v>51</v>
+      <c r="B69" s="23" t="str">
+        <f t="shared" ref="B69:F69" si="7">" "</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="C69" s="23" t="str">
+        <f t="shared" si="7"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="D69" s="23" t="str">
+        <f t="shared" si="7"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="E69" s="23" t="str">
+        <f t="shared" si="7"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="F69" s="23" t="str">
+        <f t="shared" si="7"/>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="G69" s="26" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="70" spans="1:7">
+      <c r="H69" s="37" t="str">
+        <f t="shared" si="4"/>
+        <v>'</v>
+      </c>
+      <c r="I69" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">['Mongolia', </v>
+      </c>
+      <c r="J69" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve"> ],</v>
+      </c>
+      <c r="K69" t="s">
+        <v>346</v>
+      </c>
+      <c r="L69" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12">
       <c r="A70" s="33" t="s">
         <v>152</v>
       </c>
@@ -3872,8 +5819,26 @@
       <c r="G70" s="26" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="71" spans="1:7">
+      <c r="H70" s="37" t="str">
+        <f t="shared" si="4"/>
+        <v>'</v>
+      </c>
+      <c r="I70" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">['Myanmar', </v>
+      </c>
+      <c r="J70" t="str">
+        <f t="shared" si="6"/>
+        <v>0.8],</v>
+      </c>
+      <c r="K70" t="s">
+        <v>347</v>
+      </c>
+      <c r="L70" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12">
       <c r="A71" s="33" t="s">
         <v>153</v>
       </c>
@@ -3895,8 +5860,26 @@
       <c r="G71" s="26" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="72" spans="1:7">
+      <c r="H71" s="37" t="str">
+        <f t="shared" si="4"/>
+        <v>'</v>
+      </c>
+      <c r="I71" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">['Philippines', </v>
+      </c>
+      <c r="J71" t="str">
+        <f t="shared" si="6"/>
+        <v>0.04],</v>
+      </c>
+      <c r="K71" t="s">
+        <v>348</v>
+      </c>
+      <c r="L71" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12">
       <c r="A72" s="33" t="s">
         <v>154</v>
       </c>
@@ -3918,8 +5901,26 @@
       <c r="G72" s="26" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="73" spans="1:7">
+      <c r="H72" s="37" t="str">
+        <f t="shared" si="4"/>
+        <v>'</v>
+      </c>
+      <c r="I72" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">['Republic of Korea', </v>
+      </c>
+      <c r="J72" t="str">
+        <f t="shared" si="6"/>
+        <v>0.08],</v>
+      </c>
+      <c r="K72" t="s">
+        <v>349</v>
+      </c>
+      <c r="L72" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12">
       <c r="A73" s="33" t="s">
         <v>155</v>
       </c>
@@ -3941,8 +5942,26 @@
       <c r="G73" s="26" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="74" spans="1:7">
+      <c r="H73" s="37" t="str">
+        <f t="shared" si="4"/>
+        <v>'</v>
+      </c>
+      <c r="I73" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">['Singapore', </v>
+      </c>
+      <c r="J73" t="str">
+        <f t="shared" si="6"/>
+        <v>0.33],</v>
+      </c>
+      <c r="K73" t="s">
+        <v>350</v>
+      </c>
+      <c r="L73" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12">
       <c r="A74" s="33" t="s">
         <v>156</v>
       </c>
@@ -3960,31 +5979,72 @@
       <c r="G74" s="26" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="75" spans="1:7">
+      <c r="H74" s="37" t="str">
+        <f t="shared" si="4"/>
+        <v>'</v>
+      </c>
+      <c r="I74" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">['Thailand', </v>
+      </c>
+      <c r="J74" t="str">
+        <f t="shared" si="6"/>
+        <v>0.2],</v>
+      </c>
+      <c r="K74" t="s">
+        <v>352</v>
+      </c>
+      <c r="L74" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="75" spans="1:12">
       <c r="A75" s="33" t="s">
         <v>157</v>
       </c>
-      <c r="B75" s="23" t="s">
-        <v>51</v>
-      </c>
-      <c r="C75" s="24" t="s">
-        <v>51</v>
-      </c>
-      <c r="D75" s="24" t="s">
-        <v>51</v>
-      </c>
-      <c r="E75" s="25" t="s">
-        <v>51</v>
-      </c>
-      <c r="F75" s="25" t="s">
-        <v>51</v>
+      <c r="B75" s="23" t="str">
+        <f t="shared" ref="B75:F75" si="8">" "</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="C75" s="23" t="str">
+        <f t="shared" si="8"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="D75" s="23" t="str">
+        <f t="shared" si="8"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="E75" s="23" t="str">
+        <f t="shared" si="8"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="F75" s="23" t="str">
+        <f t="shared" si="8"/>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="G75" s="26" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="76" spans="1:7">
+      <c r="H75" s="37" t="str">
+        <f t="shared" si="4"/>
+        <v>'</v>
+      </c>
+      <c r="I75" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">['Timor-Leste', </v>
+      </c>
+      <c r="J75" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve"> ],</v>
+      </c>
+      <c r="K75" t="s">
+        <v>353</v>
+      </c>
+      <c r="L75" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="76" spans="1:12">
       <c r="A76" s="33" t="s">
         <v>158</v>
       </c>
@@ -4002,8 +6062,26 @@
       <c r="G76" s="26" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="77" spans="1:7">
+      <c r="H76" s="37" t="str">
+        <f t="shared" si="4"/>
+        <v>'</v>
+      </c>
+      <c r="I76" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">['Viet Nam', </v>
+      </c>
+      <c r="J76" t="str">
+        <f t="shared" si="6"/>
+        <v>0.53],</v>
+      </c>
+      <c r="K76" t="s">
+        <v>354</v>
+      </c>
+      <c r="L76" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="77" spans="1:12">
       <c r="A77" s="33" t="s">
         <v>159</v>
       </c>
@@ -4021,8 +6099,26 @@
       <c r="G77" s="26" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="78" spans="1:7">
+      <c r="H77" s="37" t="str">
+        <f t="shared" si="4"/>
+        <v>'</v>
+      </c>
+      <c r="I77" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">['Taiwan Province of China', </v>
+      </c>
+      <c r="J77" t="str">
+        <f t="shared" si="6"/>
+        <v>0.2],</v>
+      </c>
+      <c r="K77" t="s">
+        <v>356</v>
+      </c>
+      <c r="L77" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12">
       <c r="A78" s="33" t="s">
         <v>160</v>
       </c>
@@ -4044,8 +6140,26 @@
       <c r="G78" s="26" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="79" spans="1:7">
+      <c r="H78" s="37" t="str">
+        <f t="shared" si="4"/>
+        <v>'</v>
+      </c>
+      <c r="I78" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">['Afghanistan', </v>
+      </c>
+      <c r="J78" t="str">
+        <f t="shared" si="6"/>
+        <v>2.92],</v>
+      </c>
+      <c r="K78" t="s">
+        <v>357</v>
+      </c>
+      <c r="L78" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="79" spans="1:12">
       <c r="A79" s="33" t="s">
         <v>162</v>
       </c>
@@ -4063,8 +6177,26 @@
       <c r="G79" s="26" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="80" spans="1:7">
+      <c r="H79" s="37" t="str">
+        <f t="shared" si="4"/>
+        <v>'</v>
+      </c>
+      <c r="I79" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">['Iran (Islamic Republic of)', </v>
+      </c>
+      <c r="J79" t="str">
+        <f t="shared" si="6"/>
+        <v>2.27],</v>
+      </c>
+      <c r="K79" t="s">
+        <v>359</v>
+      </c>
+      <c r="L79" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="80" spans="1:12">
       <c r="A80" s="33" t="s">
         <v>163</v>
       </c>
@@ -4086,8 +6218,26 @@
       <c r="G80" s="26" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="81" spans="1:7" ht="18" customHeight="1">
+      <c r="H80" s="37" t="str">
+        <f t="shared" si="4"/>
+        <v>'</v>
+      </c>
+      <c r="I80" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">['Israel', </v>
+      </c>
+      <c r="J80" t="str">
+        <f t="shared" si="6"/>
+        <v>0.63],</v>
+      </c>
+      <c r="K80" t="s">
+        <v>361</v>
+      </c>
+      <c r="L80" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="81" spans="1:12">
       <c r="A81" s="33" t="s">
         <v>165</v>
       </c>
@@ -4105,8 +6255,26 @@
       <c r="G81" s="26" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="82" spans="1:7">
+      <c r="H81" s="37" t="str">
+        <f t="shared" si="4"/>
+        <v>'</v>
+      </c>
+      <c r="I81" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">['Kuwait', </v>
+      </c>
+      <c r="J81" t="str">
+        <f t="shared" si="6"/>
+        <v>0.17],</v>
+      </c>
+      <c r="K81" t="s">
+        <v>362</v>
+      </c>
+      <c r="L81" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="82" spans="1:12">
       <c r="A82" s="33" t="s">
         <v>166</v>
       </c>
@@ -4124,31 +6292,72 @@
       <c r="G82" s="26" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="83" spans="1:7">
+      <c r="H82" s="37" t="str">
+        <f t="shared" si="4"/>
+        <v>'</v>
+      </c>
+      <c r="I82" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">['Lebanon', </v>
+      </c>
+      <c r="J82" t="str">
+        <f t="shared" si="6"/>
+        <v>0.2],</v>
+      </c>
+      <c r="K82" t="s">
+        <v>363</v>
+      </c>
+      <c r="L82" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="83" spans="1:12">
       <c r="A83" s="33" t="s">
         <v>167</v>
       </c>
-      <c r="B83" s="23" t="s">
-        <v>51</v>
-      </c>
-      <c r="C83" s="24" t="s">
-        <v>51</v>
-      </c>
-      <c r="D83" s="24" t="s">
-        <v>51</v>
-      </c>
-      <c r="E83" s="25" t="s">
-        <v>51</v>
-      </c>
-      <c r="F83" s="25" t="s">
-        <v>51</v>
+      <c r="B83" s="23" t="str">
+        <f t="shared" ref="B83:F83" si="9">" "</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="C83" s="23" t="str">
+        <f t="shared" si="9"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="D83" s="23" t="str">
+        <f t="shared" si="9"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="E83" s="23" t="str">
+        <f t="shared" si="9"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="F83" s="23" t="str">
+        <f t="shared" si="9"/>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="G83" s="26" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="84" spans="1:7">
+      <c r="H83" s="37" t="str">
+        <f t="shared" si="4"/>
+        <v>'</v>
+      </c>
+      <c r="I83" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">['Oman', </v>
+      </c>
+      <c r="J83" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve"> ],</v>
+      </c>
+      <c r="K83" t="s">
+        <v>364</v>
+      </c>
+      <c r="L83" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="84" spans="1:12">
       <c r="A84" s="33" t="s">
         <v>168</v>
       </c>
@@ -4170,8 +6379,26 @@
       <c r="G84" s="26" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="85" spans="1:7" ht="18" customHeight="1">
+      <c r="H84" s="37" t="str">
+        <f t="shared" si="4"/>
+        <v>'</v>
+      </c>
+      <c r="I84" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">['Pakistan', </v>
+      </c>
+      <c r="J84" t="str">
+        <f t="shared" si="6"/>
+        <v>2.4],</v>
+      </c>
+      <c r="K84" t="s">
+        <v>365</v>
+      </c>
+      <c r="L84" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="85" spans="1:12">
       <c r="A85" s="33" t="s">
         <v>170</v>
       </c>
@@ -4189,8 +6416,26 @@
       <c r="G85" s="26" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="86" spans="1:7">
+      <c r="H85" s="37" t="str">
+        <f t="shared" si="4"/>
+        <v>'</v>
+      </c>
+      <c r="I85" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">['Saudi Arabia', </v>
+      </c>
+      <c r="J85" t="str">
+        <f t="shared" si="6"/>
+        <v>0.06],</v>
+      </c>
+      <c r="K85" t="s">
+        <v>367</v>
+      </c>
+      <c r="L85" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="86" spans="1:12">
       <c r="A86" s="33" t="s">
         <v>171</v>
       </c>
@@ -4208,8 +6453,26 @@
       <c r="G86" s="26" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="87" spans="1:7">
+      <c r="H86" s="37" t="str">
+        <f t="shared" si="4"/>
+        <v>'</v>
+      </c>
+      <c r="I86" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">['Syrian Arab Republic', </v>
+      </c>
+      <c r="J86" t="str">
+        <f t="shared" si="6"/>
+        <v>0.02],</v>
+      </c>
+      <c r="K86" t="s">
+        <v>368</v>
+      </c>
+      <c r="L86" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="87" spans="1:12">
       <c r="A87" s="33" t="s">
         <v>172</v>
       </c>
@@ -4227,8 +6490,26 @@
       <c r="G87" s="26" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="88" spans="1:7" ht="18" customHeight="1">
+      <c r="H87" s="37" t="str">
+        <f t="shared" si="4"/>
+        <v>'</v>
+      </c>
+      <c r="I87" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">['United Arab Emirates', </v>
+      </c>
+      <c r="J87" t="str">
+        <f t="shared" si="6"/>
+        <v>0.02],</v>
+      </c>
+      <c r="K87" t="s">
+        <v>369</v>
+      </c>
+      <c r="L87" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="88" spans="1:12">
       <c r="A88" s="33" t="s">
         <v>173</v>
       </c>
@@ -4246,8 +6527,26 @@
       <c r="G88" s="26" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="89" spans="1:7">
+      <c r="H88" s="37" t="str">
+        <f t="shared" si="4"/>
+        <v>'</v>
+      </c>
+      <c r="I88" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">['Bangladesh', </v>
+      </c>
+      <c r="J88" t="str">
+        <f t="shared" si="6"/>
+        <v>0.4],</v>
+      </c>
+      <c r="K88" t="s">
+        <v>370</v>
+      </c>
+      <c r="L88" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="89" spans="1:12">
       <c r="A89" s="33" t="s">
         <v>174</v>
       </c>
@@ -4265,8 +6564,26 @@
       <c r="G89" s="26" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="90" spans="1:7">
+      <c r="H89" s="37" t="str">
+        <f t="shared" si="4"/>
+        <v>'</v>
+      </c>
+      <c r="I89" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">['Maldives', </v>
+      </c>
+      <c r="J89" t="str">
+        <f t="shared" si="6"/>
+        <v>1.46],</v>
+      </c>
+      <c r="K89" t="s">
+        <v>372</v>
+      </c>
+      <c r="L89" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="90" spans="1:12">
       <c r="A90" s="33" t="s">
         <v>175</v>
       </c>
@@ -4288,8 +6605,26 @@
       <c r="G90" s="26" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="91" spans="1:7">
+      <c r="H90" s="37" t="str">
+        <f t="shared" si="4"/>
+        <v>'</v>
+      </c>
+      <c r="I90" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">['Nepal', </v>
+      </c>
+      <c r="J90" t="str">
+        <f t="shared" si="6"/>
+        <v>0.24],</v>
+      </c>
+      <c r="K90" t="s">
+        <v>374</v>
+      </c>
+      <c r="L90" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="91" spans="1:12">
       <c r="A91" s="33" t="s">
         <v>176</v>
       </c>
@@ -4307,8 +6642,26 @@
       <c r="G91" s="26" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="92" spans="1:7">
+      <c r="H91" s="37" t="str">
+        <f t="shared" si="4"/>
+        <v>'</v>
+      </c>
+      <c r="I91" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">['Sri Lanka', </v>
+      </c>
+      <c r="J91" t="str">
+        <f t="shared" si="6"/>
+        <v>0.33],</v>
+      </c>
+      <c r="K91" t="s">
+        <v>376</v>
+      </c>
+      <c r="L91" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="92" spans="1:12">
       <c r="A92" s="33" t="s">
         <v>177</v>
       </c>
@@ -4326,8 +6679,26 @@
       <c r="G92" s="26" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="93" spans="1:7">
+      <c r="H92" s="37" t="str">
+        <f t="shared" si="4"/>
+        <v>'</v>
+      </c>
+      <c r="I92" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">['Belarus', </v>
+      </c>
+      <c r="J92" t="str">
+        <f t="shared" si="6"/>
+        <v>0.59],</v>
+      </c>
+      <c r="K92" t="s">
+        <v>377</v>
+      </c>
+      <c r="L92" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="93" spans="1:12">
       <c r="A93" s="33" t="s">
         <v>178</v>
       </c>
@@ -4345,8 +6716,26 @@
       <c r="G93" s="26" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="94" spans="1:7">
+      <c r="H93" s="37" t="str">
+        <f t="shared" si="4"/>
+        <v>'</v>
+      </c>
+      <c r="I93" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">['Republic of Moldova', </v>
+      </c>
+      <c r="J93" t="str">
+        <f t="shared" si="6"/>
+        <v>0.12],</v>
+      </c>
+      <c r="K93" t="s">
+        <v>379</v>
+      </c>
+      <c r="L93" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="94" spans="1:12">
       <c r="A94" s="33" t="s">
         <v>179</v>
       </c>
@@ -4368,8 +6757,26 @@
       <c r="G94" s="26" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="95" spans="1:7">
+      <c r="H94" s="37" t="str">
+        <f t="shared" si="4"/>
+        <v>'</v>
+      </c>
+      <c r="I94" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">['Russian Federation', </v>
+      </c>
+      <c r="J94" t="str">
+        <f t="shared" si="6"/>
+        <v>1.64],</v>
+      </c>
+      <c r="K94" t="s">
+        <v>380</v>
+      </c>
+      <c r="L94" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="95" spans="1:12">
       <c r="A95" s="33" t="s">
         <v>180</v>
       </c>
@@ -4387,8 +6794,26 @@
       <c r="G95" s="26" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="96" spans="1:7">
+      <c r="H95" s="37" t="str">
+        <f t="shared" si="4"/>
+        <v>'</v>
+      </c>
+      <c r="I95" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">['Ukraine', </v>
+      </c>
+      <c r="J95" t="str">
+        <f t="shared" si="6"/>
+        <v>0.91],</v>
+      </c>
+      <c r="K95" t="s">
+        <v>382</v>
+      </c>
+      <c r="L95" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="96" spans="1:12">
       <c r="A96" s="33" t="s">
         <v>181</v>
       </c>
@@ -4406,8 +6831,26 @@
       <c r="G96" s="26" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="97" spans="1:7" ht="28">
+      <c r="H96" s="37" t="str">
+        <f t="shared" si="4"/>
+        <v>'</v>
+      </c>
+      <c r="I96" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">['Albania', </v>
+      </c>
+      <c r="J96" t="str">
+        <f t="shared" si="6"/>
+        <v>0.45],</v>
+      </c>
+      <c r="K96" t="s">
+        <v>384</v>
+      </c>
+      <c r="L96" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="97" spans="1:12" ht="28">
       <c r="A97" s="33" t="s">
         <v>182</v>
       </c>
@@ -4429,8 +6872,26 @@
       <c r="G97" s="26" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="98" spans="1:7">
+      <c r="H97" s="37" t="str">
+        <f t="shared" si="4"/>
+        <v>'</v>
+      </c>
+      <c r="I97" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">['Bosnia and Herzegovina', </v>
+      </c>
+      <c r="J97" t="str">
+        <f t="shared" si="6"/>
+        <v>0.3],</v>
+      </c>
+      <c r="K97" t="s">
+        <v>386</v>
+      </c>
+      <c r="L97" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="98" spans="1:12">
       <c r="A98" s="33" t="s">
         <v>183</v>
       </c>
@@ -4448,8 +6909,26 @@
       <c r="G98" s="26" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="99" spans="1:7">
+      <c r="H98" s="37" t="str">
+        <f t="shared" si="4"/>
+        <v>'</v>
+      </c>
+      <c r="I98" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">['Bulgaria', </v>
+      </c>
+      <c r="J98" t="str">
+        <f t="shared" si="6"/>
+        <v>0.51],</v>
+      </c>
+      <c r="K98" t="s">
+        <v>387</v>
+      </c>
+      <c r="L98" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="99" spans="1:12">
       <c r="A99" s="33" t="s">
         <v>184</v>
       </c>
@@ -4471,8 +6950,26 @@
       <c r="G99" s="26" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="100" spans="1:7">
+      <c r="H99" s="37" t="str">
+        <f t="shared" si="4"/>
+        <v>'</v>
+      </c>
+      <c r="I99" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">['Croatia', </v>
+      </c>
+      <c r="J99" t="str">
+        <f t="shared" si="6"/>
+        <v>0.36],</v>
+      </c>
+      <c r="K99" t="s">
+        <v>389</v>
+      </c>
+      <c r="L99" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="100" spans="1:12">
       <c r="A100" s="33" t="s">
         <v>186</v>
       </c>
@@ -4490,8 +6987,26 @@
       <c r="G100" s="26" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="101" spans="1:7">
+      <c r="H100" s="37" t="str">
+        <f t="shared" si="4"/>
+        <v>'</v>
+      </c>
+      <c r="I100" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">['The former Yugoslav Republic of Macedonia', </v>
+      </c>
+      <c r="J100" t="str">
+        <f t="shared" si="6"/>
+        <v>0.5],</v>
+      </c>
+      <c r="K100" t="s">
+        <v>391</v>
+      </c>
+      <c r="L100" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="101" spans="1:12">
       <c r="A101" s="33" t="s">
         <v>187</v>
       </c>
@@ -4509,8 +7024,26 @@
       <c r="G101" s="26" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="102" spans="1:7" ht="18" customHeight="1">
+      <c r="H101" s="37" t="str">
+        <f t="shared" si="4"/>
+        <v>'</v>
+      </c>
+      <c r="I101" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">['Romania', </v>
+      </c>
+      <c r="J101" t="str">
+        <f t="shared" si="6"/>
+        <v>0.11],</v>
+      </c>
+      <c r="K101" t="s">
+        <v>392</v>
+      </c>
+      <c r="L101" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="102" spans="1:12">
       <c r="A102" s="33" t="s">
         <v>188</v>
       </c>
@@ -4532,8 +7065,26 @@
       <c r="G102" s="26" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="103" spans="1:7">
+      <c r="H102" s="37" t="str">
+        <f t="shared" si="4"/>
+        <v>'</v>
+      </c>
+      <c r="I102" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">['Turkey', </v>
+      </c>
+      <c r="J102" t="str">
+        <f t="shared" si="6"/>
+        <v>0.03],</v>
+      </c>
+      <c r="K102" t="s">
+        <v>393</v>
+      </c>
+      <c r="L102" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="103" spans="1:12">
       <c r="A103" s="33" t="s">
         <v>189</v>
       </c>
@@ -4555,8 +7106,26 @@
       <c r="G103" s="26" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="104" spans="1:7">
+      <c r="H103" s="37" t="str">
+        <f t="shared" si="4"/>
+        <v>'</v>
+      </c>
+      <c r="I103" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">['Serbia', </v>
+      </c>
+      <c r="J103" t="str">
+        <f t="shared" si="6"/>
+        <v>0.28],</v>
+      </c>
+      <c r="K103" t="s">
+        <v>394</v>
+      </c>
+      <c r="L103" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="104" spans="1:12">
       <c r="A104" s="33" t="s">
         <v>190</v>
       </c>
@@ -4578,8 +7147,26 @@
       <c r="G104" s="26" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="105" spans="1:7">
+      <c r="H104" s="37" t="str">
+        <f t="shared" si="4"/>
+        <v>'</v>
+      </c>
+      <c r="I104" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">['Austria', </v>
+      </c>
+      <c r="J104" t="str">
+        <f t="shared" si="6"/>
+        <v>0.53],</v>
+      </c>
+      <c r="K104" t="s">
+        <v>395</v>
+      </c>
+      <c r="L104" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="105" spans="1:12">
       <c r="A105" s="33" t="s">
         <v>191</v>
       </c>
@@ -4597,8 +7184,26 @@
       <c r="G105" s="26" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="106" spans="1:7">
+      <c r="H105" s="37" t="str">
+        <f t="shared" si="4"/>
+        <v>'</v>
+      </c>
+      <c r="I105" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">['Belgium', </v>
+      </c>
+      <c r="J105" t="str">
+        <f t="shared" si="6"/>
+        <v>0.2],</v>
+      </c>
+      <c r="K105" t="s">
+        <v>396</v>
+      </c>
+      <c r="L105" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="106" spans="1:12">
       <c r="A106" s="33" t="s">
         <v>192</v>
       </c>
@@ -4620,8 +7225,26 @@
       <c r="G106" s="26" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="107" spans="1:7">
+      <c r="H106" s="37" t="str">
+        <f t="shared" si="4"/>
+        <v>'</v>
+      </c>
+      <c r="I106" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">['Cyprus', </v>
+      </c>
+      <c r="J106" t="str">
+        <f t="shared" si="6"/>
+        <v>0.12],</v>
+      </c>
+      <c r="K106" t="s">
+        <v>397</v>
+      </c>
+      <c r="L106" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="107" spans="1:12">
       <c r="A107" s="33" t="s">
         <v>193</v>
       </c>
@@ -4639,8 +7262,26 @@
       <c r="G107" s="26" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="108" spans="1:7">
+      <c r="H107" s="37" t="str">
+        <f t="shared" si="4"/>
+        <v>'</v>
+      </c>
+      <c r="I107" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">['Czech Republic', </v>
+      </c>
+      <c r="J107" t="str">
+        <f t="shared" si="6"/>
+        <v>2.7],</v>
+      </c>
+      <c r="K107" t="s">
+        <v>398</v>
+      </c>
+      <c r="L107" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="108" spans="1:12">
       <c r="A108" s="33" t="s">
         <v>194</v>
       </c>
@@ -4662,8 +7303,26 @@
       <c r="G108" s="26" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="109" spans="1:7">
+      <c r="H108" s="37" t="str">
+        <f t="shared" si="4"/>
+        <v>'</v>
+      </c>
+      <c r="I108" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">['Denmark', </v>
+      </c>
+      <c r="J108" t="str">
+        <f t="shared" si="6"/>
+        <v>0.52],</v>
+      </c>
+      <c r="K108" t="s">
+        <v>400</v>
+      </c>
+      <c r="L108" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="109" spans="1:12">
       <c r="A109" s="33" t="s">
         <v>195</v>
       </c>
@@ -4681,8 +7340,26 @@
       <c r="G109" s="26" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="110" spans="1:7">
+      <c r="H109" s="37" t="str">
+        <f t="shared" si="4"/>
+        <v>'</v>
+      </c>
+      <c r="I109" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">['Estonia', </v>
+      </c>
+      <c r="J109" t="str">
+        <f t="shared" si="6"/>
+        <v>1.53],</v>
+      </c>
+      <c r="K109" t="s">
+        <v>402</v>
+      </c>
+      <c r="L109" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="110" spans="1:12">
       <c r="A110" s="33" t="s">
         <v>196</v>
       </c>
@@ -4700,8 +7377,26 @@
       <c r="G110" s="26" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="111" spans="1:7">
+      <c r="H110" s="37" t="str">
+        <f t="shared" si="4"/>
+        <v>'</v>
+      </c>
+      <c r="I110" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">['Finland', </v>
+      </c>
+      <c r="J110" t="str">
+        <f t="shared" si="6"/>
+        <v>0.6],</v>
+      </c>
+      <c r="K110" t="s">
+        <v>404</v>
+      </c>
+      <c r="L110" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="111" spans="1:12">
       <c r="A111" s="33" t="s">
         <v>197</v>
       </c>
@@ -4719,8 +7414,26 @@
       <c r="G111" s="26" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="112" spans="1:7">
+      <c r="H111" s="37" t="str">
+        <f t="shared" si="4"/>
+        <v>'</v>
+      </c>
+      <c r="I111" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">['France', </v>
+      </c>
+      <c r="J111" t="str">
+        <f t="shared" si="6"/>
+        <v>0.49],</v>
+      </c>
+      <c r="K111" t="s">
+        <v>405</v>
+      </c>
+      <c r="L111" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="112" spans="1:12">
       <c r="A112" s="33" t="s">
         <v>198</v>
       </c>
@@ -4738,8 +7451,26 @@
       <c r="G112" s="26" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="113" spans="1:7">
+      <c r="H112" s="37" t="str">
+        <f t="shared" si="4"/>
+        <v>'</v>
+      </c>
+      <c r="I112" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">['Germany', </v>
+      </c>
+      <c r="J112" t="str">
+        <f t="shared" si="6"/>
+        <v>0.4],</v>
+      </c>
+      <c r="K112" t="s">
+        <v>407</v>
+      </c>
+      <c r="L112" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="113" spans="1:12">
       <c r="A113" s="33" t="s">
         <v>200</v>
       </c>
@@ -4761,8 +7492,26 @@
       <c r="G113" s="26" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="114" spans="1:7">
+      <c r="H113" s="37" t="str">
+        <f t="shared" si="4"/>
+        <v>'</v>
+      </c>
+      <c r="I113" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">['Greece', </v>
+      </c>
+      <c r="J113" t="str">
+        <f t="shared" si="6"/>
+        <v>0.29],</v>
+      </c>
+      <c r="K113" t="s">
+        <v>408</v>
+      </c>
+      <c r="L113" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="114" spans="1:12">
       <c r="A114" s="33" t="s">
         <v>201</v>
       </c>
@@ -4784,8 +7533,26 @@
       <c r="G114" s="28" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="115" spans="1:7">
+      <c r="H114" s="37" t="str">
+        <f t="shared" si="4"/>
+        <v>'</v>
+      </c>
+      <c r="I114" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">['Hungary', </v>
+      </c>
+      <c r="J114" t="str">
+        <f t="shared" si="6"/>
+        <v>0.05],</v>
+      </c>
+      <c r="K114" t="s">
+        <v>410</v>
+      </c>
+      <c r="L114" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="115" spans="1:12">
       <c r="A115" s="33" t="s">
         <v>203</v>
       </c>
@@ -4803,8 +7570,26 @@
       <c r="G115" s="26" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="116" spans="1:7">
+      <c r="H115" s="37" t="str">
+        <f t="shared" si="4"/>
+        <v>'</v>
+      </c>
+      <c r="I115" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">['Iceland', </v>
+      </c>
+      <c r="J115" t="str">
+        <f t="shared" si="6"/>
+        <v>0.4],</v>
+      </c>
+      <c r="K115" t="s">
+        <v>411</v>
+      </c>
+      <c r="L115" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="116" spans="1:12">
       <c r="A116" s="33" t="s">
         <v>204</v>
       </c>
@@ -4826,8 +7611,26 @@
       <c r="G116" s="26" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="117" spans="1:7">
+      <c r="H116" s="37" t="str">
+        <f t="shared" si="4"/>
+        <v>'</v>
+      </c>
+      <c r="I116" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">['Ireland', </v>
+      </c>
+      <c r="J116" t="str">
+        <f t="shared" si="6"/>
+        <v>0.72],</v>
+      </c>
+      <c r="K116" t="s">
+        <v>412</v>
+      </c>
+      <c r="L116" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="117" spans="1:12">
       <c r="A117" s="33" t="s">
         <v>205</v>
       </c>
@@ -4849,8 +7652,26 @@
       <c r="G117" s="26" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="118" spans="1:7">
+      <c r="H117" s="37" t="str">
+        <f t="shared" si="4"/>
+        <v>'</v>
+      </c>
+      <c r="I117" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">['Italy', </v>
+      </c>
+      <c r="J117" t="str">
+        <f t="shared" si="6"/>
+        <v>0.45],</v>
+      </c>
+      <c r="K117" t="s">
+        <v>414</v>
+      </c>
+      <c r="L117" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="118" spans="1:12">
       <c r="A118" s="33" t="s">
         <v>206</v>
       </c>
@@ -4868,8 +7689,26 @@
       <c r="G118" s="26" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="119" spans="1:7">
+      <c r="H118" s="37" t="str">
+        <f t="shared" si="4"/>
+        <v>'</v>
+      </c>
+      <c r="I118" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">['Latvia', </v>
+      </c>
+      <c r="J118" t="str">
+        <f t="shared" si="6"/>
+        <v>0.66],</v>
+      </c>
+      <c r="K118" t="s">
+        <v>415</v>
+      </c>
+      <c r="L118" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="119" spans="1:12">
       <c r="A119" s="33" t="s">
         <v>208</v>
       </c>
@@ -4887,8 +7726,26 @@
       <c r="G119" s="26" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="120" spans="1:7">
+      <c r="H119" s="37" t="str">
+        <f t="shared" si="4"/>
+        <v>'</v>
+      </c>
+      <c r="I119" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">['Liechtenstein', </v>
+      </c>
+      <c r="J119" t="str">
+        <f t="shared" si="6"/>
+        <v>0.2],</v>
+      </c>
+      <c r="K119" t="s">
+        <v>417</v>
+      </c>
+      <c r="L119" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="120" spans="1:12">
       <c r="A120" s="33" t="s">
         <v>209</v>
       </c>
@@ -4910,8 +7767,26 @@
       <c r="G120" s="26" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="121" spans="1:7">
+      <c r="H120" s="37" t="str">
+        <f t="shared" si="4"/>
+        <v>'</v>
+      </c>
+      <c r="I120" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">['Lithuania', </v>
+      </c>
+      <c r="J120" t="str">
+        <f t="shared" si="6"/>
+        <v>0.24],</v>
+      </c>
+      <c r="K120" t="s">
+        <v>418</v>
+      </c>
+      <c r="L120" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="121" spans="1:12">
       <c r="A121" s="33" t="s">
         <v>210</v>
       </c>
@@ -4929,8 +7804,26 @@
       <c r="G121" s="26" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="122" spans="1:7">
+      <c r="H121" s="37" t="str">
+        <f t="shared" si="4"/>
+        <v>'</v>
+      </c>
+      <c r="I121" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">['Luxembourg', </v>
+      </c>
+      <c r="J121" t="str">
+        <f t="shared" si="6"/>
+        <v>0.59],</v>
+      </c>
+      <c r="K121" t="s">
+        <v>419</v>
+      </c>
+      <c r="L121" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="122" spans="1:12">
       <c r="A122" s="33" t="s">
         <v>211</v>
       </c>
@@ -4952,31 +7845,72 @@
       <c r="G122" s="26" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="123" spans="1:7">
+      <c r="H122" s="37" t="str">
+        <f t="shared" si="4"/>
+        <v>'</v>
+      </c>
+      <c r="I122" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">['Malta', </v>
+      </c>
+      <c r="J122" t="str">
+        <f t="shared" si="6"/>
+        <v>0.62],</v>
+      </c>
+      <c r="K122" t="s">
+        <v>420</v>
+      </c>
+      <c r="L122" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="123" spans="1:12">
       <c r="A123" s="33" t="s">
         <v>212</v>
       </c>
-      <c r="B123" s="23" t="s">
-        <v>51</v>
-      </c>
-      <c r="C123" s="24" t="s">
-        <v>51</v>
-      </c>
-      <c r="D123" s="24" t="s">
-        <v>51</v>
-      </c>
-      <c r="E123" s="25" t="s">
-        <v>51</v>
-      </c>
-      <c r="F123" s="25" t="s">
-        <v>51</v>
+      <c r="B123" s="23" t="str">
+        <f t="shared" ref="B123:F123" si="10">" "</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="C123" s="23" t="str">
+        <f t="shared" si="10"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="D123" s="23" t="str">
+        <f t="shared" si="10"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="E123" s="23" t="str">
+        <f t="shared" si="10"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="F123" s="23" t="str">
+        <f t="shared" si="10"/>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="G123" s="26" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="124" spans="1:7">
+      <c r="H123" s="37" t="str">
+        <f t="shared" si="4"/>
+        <v>'</v>
+      </c>
+      <c r="I123" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">['Monaco', </v>
+      </c>
+      <c r="J123" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve"> ],</v>
+      </c>
+      <c r="K123" t="s">
+        <v>422</v>
+      </c>
+      <c r="L123" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="124" spans="1:12">
       <c r="A124" s="33" t="s">
         <v>213</v>
       </c>
@@ -4998,8 +7932,26 @@
       <c r="G124" s="26" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="125" spans="1:7">
+      <c r="H124" s="37" t="str">
+        <f t="shared" si="4"/>
+        <v>'</v>
+      </c>
+      <c r="I124" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">['Netherlands', </v>
+      </c>
+      <c r="J124" t="str">
+        <f t="shared" si="6"/>
+        <v>0.13],</v>
+      </c>
+      <c r="K124" t="s">
+        <v>423</v>
+      </c>
+      <c r="L124" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="125" spans="1:12">
       <c r="A125" s="33" t="s">
         <v>214</v>
       </c>
@@ -5021,8 +7973,26 @@
       <c r="G125" s="26" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="126" spans="1:7">
+      <c r="H125" s="37" t="str">
+        <f t="shared" si="4"/>
+        <v>'</v>
+      </c>
+      <c r="I125" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">['Norway', </v>
+      </c>
+      <c r="J125" t="str">
+        <f t="shared" si="6"/>
+        <v>0.3],</v>
+      </c>
+      <c r="K125" t="s">
+        <v>424</v>
+      </c>
+      <c r="L125" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="126" spans="1:12">
       <c r="A126" s="33" t="s">
         <v>215</v>
       </c>
@@ -5040,8 +8010,26 @@
       <c r="G126" s="26" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="127" spans="1:7">
+      <c r="H126" s="37" t="str">
+        <f t="shared" si="4"/>
+        <v>'</v>
+      </c>
+      <c r="I126" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">['Poland', </v>
+      </c>
+      <c r="J126" t="str">
+        <f t="shared" si="6"/>
+        <v>0.1],</v>
+      </c>
+      <c r="K126" t="s">
+        <v>425</v>
+      </c>
+      <c r="L126" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="127" spans="1:12">
       <c r="A127" s="33" t="s">
         <v>216</v>
       </c>
@@ -5059,8 +8047,26 @@
       <c r="G127" s="26" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="128" spans="1:7">
+      <c r="H127" s="37" t="str">
+        <f t="shared" si="4"/>
+        <v>'</v>
+      </c>
+      <c r="I127" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">['Portugal', </v>
+      </c>
+      <c r="J127" t="str">
+        <f t="shared" si="6"/>
+        <v>0.29],</v>
+      </c>
+      <c r="K127" t="s">
+        <v>426</v>
+      </c>
+      <c r="L127" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="128" spans="1:12">
       <c r="A128" s="33" t="s">
         <v>217</v>
       </c>
@@ -5082,8 +8088,26 @@
       <c r="G128" s="26" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="129" spans="1:7">
+      <c r="H128" s="37" t="str">
+        <f t="shared" si="4"/>
+        <v>'</v>
+      </c>
+      <c r="I128" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">['Slovenia', </v>
+      </c>
+      <c r="J128" t="str">
+        <f t="shared" si="6"/>
+        <v>0.44],</v>
+      </c>
+      <c r="K128" t="s">
+        <v>427</v>
+      </c>
+      <c r="L128" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="129" spans="1:12">
       <c r="A129" s="33" t="s">
         <v>218</v>
       </c>
@@ -5105,8 +8129,26 @@
       <c r="G129" s="26" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="130" spans="1:7">
+      <c r="H129" s="37" t="str">
+        <f t="shared" si="4"/>
+        <v>'</v>
+      </c>
+      <c r="I129" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">['Slovakia', </v>
+      </c>
+      <c r="J129" t="str">
+        <f t="shared" si="6"/>
+        <v>0.13],</v>
+      </c>
+      <c r="K129" t="s">
+        <v>428</v>
+      </c>
+      <c r="L129" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="130" spans="1:12">
       <c r="A130" s="33" t="s">
         <v>219</v>
       </c>
@@ -5128,8 +8170,26 @@
       <c r="G130" s="26" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="131" spans="1:7">
+      <c r="H130" s="37" t="str">
+        <f t="shared" si="4"/>
+        <v>'</v>
+      </c>
+      <c r="I130" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">['Spain', </v>
+      </c>
+      <c r="J130" t="str">
+        <f t="shared" si="6"/>
+        <v>0.23],</v>
+      </c>
+      <c r="K130" t="s">
+        <v>429</v>
+      </c>
+      <c r="L130" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="131" spans="1:12">
       <c r="A131" s="33" t="s">
         <v>221</v>
       </c>
@@ -5151,8 +8211,26 @@
       <c r="G131" s="26" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="132" spans="1:7">
+      <c r="H131" s="37" t="str">
+        <f t="shared" ref="H131:H137" si="11">"'"</f>
+        <v>'</v>
+      </c>
+      <c r="I131" t="str">
+        <f t="shared" ref="I131:I137" si="12">CONCATENATE("[",H131,A131,H131,", ")</f>
+        <v xml:space="preserve">['Sweden', </v>
+      </c>
+      <c r="J131" t="str">
+        <f t="shared" ref="J131:J137" si="13">CONCATENATE(B131,"],")</f>
+        <v>0.23],</v>
+      </c>
+      <c r="K131" t="s">
+        <v>430</v>
+      </c>
+      <c r="L131" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="132" spans="1:12">
       <c r="A132" s="33" t="s">
         <v>222</v>
       </c>
@@ -5170,8 +8248,26 @@
       <c r="G132" s="26" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="133" spans="1:7">
+      <c r="H132" s="37" t="str">
+        <f t="shared" si="11"/>
+        <v>'</v>
+      </c>
+      <c r="I132" t="str">
+        <f t="shared" si="12"/>
+        <v xml:space="preserve">['Switzerland', </v>
+      </c>
+      <c r="J132" t="str">
+        <f t="shared" si="13"/>
+        <v>0.1],</v>
+      </c>
+      <c r="K132" t="s">
+        <v>431</v>
+      </c>
+      <c r="L132" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="133" spans="1:12">
       <c r="A133" s="33" t="s">
         <v>223</v>
       </c>
@@ -5193,8 +8289,26 @@
       <c r="G133" s="28" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="134" spans="1:7">
+      <c r="H133" s="37" t="str">
+        <f t="shared" si="11"/>
+        <v>'</v>
+      </c>
+      <c r="I133" t="str">
+        <f t="shared" si="12"/>
+        <v xml:space="preserve">['United Kingdom (England and Wales)', </v>
+      </c>
+      <c r="J133" t="str">
+        <f t="shared" si="13"/>
+        <v>0.73],</v>
+      </c>
+      <c r="K133" t="s">
+        <v>432</v>
+      </c>
+      <c r="L133" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="134" spans="1:12">
       <c r="A134" s="33" t="s">
         <v>226</v>
       </c>
@@ -5216,8 +8330,26 @@
       <c r="G134" s="28" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="135" spans="1:7">
+      <c r="H134" s="37" t="str">
+        <f t="shared" si="11"/>
+        <v>'</v>
+      </c>
+      <c r="I134" t="str">
+        <f t="shared" si="12"/>
+        <v xml:space="preserve">['United Kingdom (Northern Ireland)', </v>
+      </c>
+      <c r="J134" t="str">
+        <f t="shared" si="13"/>
+        <v>0.13],</v>
+      </c>
+      <c r="K134" t="s">
+        <v>434</v>
+      </c>
+      <c r="L134" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="135" spans="1:12">
       <c r="A135" s="33" t="s">
         <v>228</v>
       </c>
@@ -5239,8 +8371,26 @@
       <c r="G135" s="28" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="136" spans="1:7" ht="18" customHeight="1">
+      <c r="H135" s="37" t="str">
+        <f t="shared" si="11"/>
+        <v>'</v>
+      </c>
+      <c r="I135" t="str">
+        <f t="shared" si="12"/>
+        <v xml:space="preserve">['United Kingdom (Scotland)', </v>
+      </c>
+      <c r="J135" t="str">
+        <f t="shared" si="13"/>
+        <v>1.71],</v>
+      </c>
+      <c r="K135" t="s">
+        <v>435</v>
+      </c>
+      <c r="L135" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="136" spans="1:12">
       <c r="A136" s="33" t="s">
         <v>230</v>
       </c>
@@ -5262,8 +8412,26 @@
       <c r="G136" s="26" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="137" spans="1:7">
+      <c r="H136" s="37" t="str">
+        <f t="shared" si="11"/>
+        <v>'</v>
+      </c>
+      <c r="I136" t="str">
+        <f t="shared" si="12"/>
+        <v xml:space="preserve">['Australia', </v>
+      </c>
+      <c r="J136" t="str">
+        <f t="shared" si="13"/>
+        <v>3.4],</v>
+      </c>
+      <c r="K136" t="s">
+        <v>437</v>
+      </c>
+      <c r="L136" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="137" spans="1:12">
       <c r="A137" s="34" t="s">
         <v>231</v>
       </c>
@@ -5285,29 +8453,28 @@
       <c r="G137" s="32" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="138" spans="1:7">
+      <c r="H137" s="37" t="str">
+        <f t="shared" si="11"/>
+        <v>'</v>
+      </c>
+      <c r="I137" t="str">
+        <f t="shared" si="12"/>
+        <v xml:space="preserve">['New Zealand', </v>
+      </c>
+      <c r="J137" t="str">
+        <f t="shared" si="13"/>
+        <v>1.1],</v>
+      </c>
+      <c r="K137" t="s">
+        <v>439</v>
+      </c>
+      <c r="L137" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="138" spans="1:12">
       <c r="A138" s="18"/>
     </row>
-    <row r="143" spans="1:7" ht="15" customHeight="1"/>
-    <row r="144" spans="1:7" ht="15" customHeight="1"/>
-    <row r="145" ht="15" customHeight="1"/>
-    <row r="146" ht="15" customHeight="1"/>
-    <row r="147" ht="15" customHeight="1"/>
-    <row r="148" ht="15" customHeight="1"/>
-    <row r="149" ht="15" customHeight="1"/>
-    <row r="150" ht="15" customHeight="1"/>
-    <row r="151" ht="15" customHeight="1"/>
-    <row r="152" ht="15" customHeight="1"/>
-    <row r="153" ht="15" customHeight="1"/>
-    <row r="154" ht="15" customHeight="1"/>
-    <row r="155" ht="23" customHeight="1"/>
-    <row r="157" ht="15" customHeight="1"/>
-    <row r="158" ht="15" customHeight="1"/>
-    <row r="159" ht="15" customHeight="1"/>
-    <row r="160" ht="15" customHeight="1"/>
-    <row r="161" ht="15" customHeight="1"/>
-    <row r="162" ht="15" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
D3 stacked chart implemented
</commit_message>
<xml_diff>
--- a/2 - Heroin/h.xlsx
+++ b/2 - Heroin/h.xlsx
@@ -3866,7 +3866,7 @@
   <dimension ref="A1:H41"/>
   <sheetViews>
     <sheetView topLeftCell="A15" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4673,12 +4673,13 @@
   <dimension ref="A1:H36"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="2" max="2" width="21.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" hidden="1">

</xml_diff>